<commit_message>
Giải thích hóa quyền điền trạch
</commit_message>
<xml_diff>
--- a/LuanHuynhDe.xlsx
+++ b/LuanHuynhDe.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="29029"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24334"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="E:\Tuvi\TuVi\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5B71092-6C42-4928-B942-875C977EF4BA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473E174A-CD06-4FA2-A0C3-D37FE5871484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3168" uniqueCount="1743">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6346" uniqueCount="1752">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -5260,6 +5260,33 @@
   </si>
   <si>
     <t>Vị trí cung Huynh Đệ so với ngũ hành Mệnh: Bại địa</t>
+  </si>
+  <si>
+    <t>Trường hợp Hóa Quyền rơi vào cung huynh đệ, là chủ về tính quyền uy, lực hành động, như vậy có thể biết anh em có uy hơn mệnh tạo, cũng tích cực hơn mệnh tạo, đồng thời các quyết định lớn nhỏ trong nhà cung đều do anh em làm chủ. Hóa Quyền còn đại biểu cho kĩ năng chuyên nghiệp và năng lực chuyên môn, cho nên anh em của mệnh tạo phần nhiều là người có kĩ năng chuyên nghiệp. Nếu lấy cung huynh đệ lập thái cực mà Hóa Lộc và Hóa Kị nhập "ngà cung", thì anh em phần nhiều là người có địa vị xã hội.</t>
+  </si>
+  <si>
+    <t>Tiếp theo trên, Hóa Quyền ở cung huynh đệ, ở trong tuyến "huynh nô" là có ý so sánh đẳng cấp. Cho nên những người mệnh tạo giao du phần nhiều là người có địa vị xã hội cao hơn mệnh tạo. Do đó có thể suy ra mệnh tạo có quan hệ giao tế khá tốt, mà địa vị xã hội của mệnh tạo cũng nhờ đó mà được nâng lên. Nhưng vì Hóa Quyền ở cung huynh đệ, nên mệnh tạo thiếu năng lực hành động, thiếu thực tiễn; phần nhiều còn trông cậy vào anh em. Muốn biết anh em trợ giúp có thực chất hay không thì phải xem tình hình Hóa Lộc, Hóa Kị và cung huynh đệ phi hóa như thế nào.</t>
+  </si>
+  <si>
+    <t>Vì Hóa Quyền ở cung huynh đệ, tất nhiên có tượng đè ép, nên phần nhiều mệnh tạo có anh trai hoặc chị gái, mà không phải là trường nam hay trường nữ (có thể là anh hay chị yếu mạng). Bản chất của Hóa Quyền là "hòa" chủ về có biến động nhanh chóng, nóng bòng. Trường hợp Hóa Quyền ở cung huynh đệ, thì sự qua lại giữa mệnh tạo và anh em khá nhiệt tình, dù quan hệ có thay đổi cũng không đến nỗi có chiến tranh lạnh. Cung huynh đệ là "kho" của cung tài bạch, Hóa Quyền ở "kho tiền" bản thân mệnh tạo điều độ tiền bạc khá nhanh, vì vậy phải có tiền lưu chuyển ở trong "kho", tất nhiên cũng có của cải đế sử dụng. Đặc biệt là người có Hóa Lộc và Hóa Kị [năm sinh] nhập "ngã cung", phần nhiều không cần lo lắng về tiền bạc, của cải.</t>
+  </si>
+  <si>
+    <t>Tình hình điều độ tiền bạc sẽ mỗi lúc càng ít đi, càng khó khăn hơn</t>
+  </si>
+  <si>
+    <t>Tình hình điều độ tiền bạc sẽ mỗi lúc càng ít đi, càng khó khăn hơn, việc phải lấy tiền đằng đông đắp vào đằng tây, xoay sở tiền cực nhọc</t>
+  </si>
+  <si>
+    <t>Là chủ về thế chất mạnh mẽ dẻo dai, có thể chịu đụng sự đả kích từ bên ngoài của Hóa Kị, thường thường còn có lực đề kháng đối với tai hại bất ngờ.</t>
+  </si>
+  <si>
+    <t>Là chủ về thế chất mạnh mẽ dẻo dai, có thể chịu đụng sự đả kích từ bên ngoài của Hóa Kị, thường thường còn có lực đề kháng đối với tai hại bất ngờ. Cung vị khí số của cung tật ách cũng là cung dùng để tìm hiểu tâm tư sâu kín. Hóa Quyền ở cung huynh đệ, chủ về tâm tư sâu kín của mệnh tạo vận tác một cách mau lẹ, trong đó mệnh tạo còn có kì vọng tự lập tự cường, và ý đồ phấn đấu đi lên (nhưng những kì vọng và ý đồ của mệnh tạo sẽ khó thực hiện, vì Hóa Quyền ở "tha cung" nên sức tưởng tượng lớn hơn lực tạo tác).</t>
+  </si>
+  <si>
+    <t>Cung huynh đệ ở giữa cung mệnh và cung phu thê, là cầu nối giữa mệnh tạo với người phối ngẫu, có Hóa Quyền, là chủ về mệnh tạo đang ở trong giai đoạn nói chuyện yêu đương, tác động lẫn nhau dồn dập, cũng không thiếu sự tranh chấp; cũng vì là cung vị cầu nối, nên còn có hàm ý mệnh tạo vì tình yêu mà phải bôn ba ngược xuôi.  Là cung vị cầu nối, mà còn là cung vị đại biểu cho mẹ, nên có thể xem là gia đình chồng hay gia đình vợ phát huy sức ảnh hưởng của mình, cũng có ý tượng xen vào cuộc sống hôn nhân của mệnh tạo; hơn nữa, lấy khái niệm so sánh để luận, cung huynh đệ có Hóa Quyền thì gia đình chồng hay gia đình vợ có quyền uy tuyệt đối, cũng có thể vì vậy mà cuộc sống hôn nhân của mệnh tạo không được yên ổn. Vì cung huynh đệ là cung vị đại biểu cho mẹ, do đó mẹ của mệnh tạo cũng sức ảnh hưởng mạnh.</t>
+  </si>
+  <si>
+    <t>Cung huynh đệ là cung vị biểu hiện của cung điền trạch, có Hóa Quyền, thì đối với việc trang hoàng trong nhà mệnh tạo có yêu cầu thực dụng, có phong cách; hơn nữa, vì Hóa Quyền chủ về biến động lớn, nên gia cụ trong nhà hay thay đổi hoặc dời chuyển, và thường có khách đến thăm; vả lại, không loại trừ trường hợp chính bản thân mệnh tạo cũng thường hay dời chuyển.</t>
   </si>
 </sst>
 </file>
@@ -5614,15 +5641,21 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:G1584"/>
+  <dimension ref="A1:H1584"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1560" workbookViewId="0">
-      <selection activeCell="E1571" sqref="E1571"/>
+    <sheetView tabSelected="1" topLeftCell="A1185" workbookViewId="0">
+      <selection activeCell="C1193" sqref="C1193"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
     <col min="1" max="2" width="72.5703125" style="1" customWidth="1"/>
+    <col min="3" max="3" width="55.42578125" customWidth="1"/>
+    <col min="4" max="4" width="49.7109375" customWidth="1"/>
+    <col min="5" max="5" width="46.42578125" customWidth="1"/>
+    <col min="6" max="6" width="39.42578125" customWidth="1"/>
+    <col min="7" max="7" width="39.7109375" customWidth="1"/>
+    <col min="8" max="8" width="23.7109375" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -10145,7 +10178,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="566" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A566" s="1" t="s">
         <v>596</v>
       </c>
@@ -11310,7 +11343,7 @@
         <v>741</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>741</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
@@ -11334,7 +11367,7 @@
         <v>744</v>
       </c>
       <c r="B714" s="1" t="s">
-        <v>744</v>
+        <v>1747</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
@@ -13737,7 +13770,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="1015" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1015" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
         <v>1030</v>
       </c>
@@ -13961,7 +13994,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="1043" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1043" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1043" s="1" t="s">
         <v>1058</v>
       </c>
@@ -14073,7 +14106,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="1057" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1057" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1057" s="1" t="s">
         <v>1072</v>
       </c>
@@ -15097,7 +15130,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="1185" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1185" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1185" s="1" t="s">
         <v>1182</v>
       </c>
@@ -15105,7 +15138,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="1186" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1186" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1186" s="1" t="s">
         <v>1183</v>
       </c>
@@ -15113,7 +15146,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="1187" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1187" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1187" s="1" t="s">
         <v>1184</v>
       </c>
@@ -15121,7 +15154,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="1188" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1188" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1188" s="1" t="s">
         <v>1185</v>
       </c>
@@ -15129,7 +15162,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="1189" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1189" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1189" s="1" t="s">
         <v>1186</v>
       </c>
@@ -15137,7 +15170,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="1190" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1190" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1190" s="1" t="s">
         <v>1187</v>
       </c>
@@ -15145,7 +15178,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="1191" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1191" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1191" s="1" t="s">
         <v>1188</v>
       </c>
@@ -15153,7 +15186,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="1192" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="1192" spans="1:8" ht="60" x14ac:dyDescent="0.25">
       <c r="A1192" s="1" t="s">
         <v>1189</v>
       </c>
@@ -15161,15 +15194,33 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="1193" spans="1:2" ht="60" x14ac:dyDescent="0.25">
+    <row r="1193" spans="1:8" ht="315" x14ac:dyDescent="0.25">
       <c r="A1193" s="1" t="s">
         <v>1190</v>
       </c>
       <c r="B1193" s="1" t="s">
         <v>1638</v>
       </c>
-    </row>
-    <row r="1194" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+      <c r="C1193" s="1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="D1193" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="E1193" s="1" t="s">
+        <v>1745</v>
+      </c>
+      <c r="F1193" s="1" t="s">
+        <v>1749</v>
+      </c>
+      <c r="G1193" s="1" t="s">
+        <v>1750</v>
+      </c>
+      <c r="H1193" s="1" t="s">
+        <v>1751</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1194" s="1" t="s">
         <v>1191</v>
       </c>
@@ -15177,7 +15228,7 @@
         <v>1639</v>
       </c>
     </row>
-    <row r="1195" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1195" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1195" s="1" t="s">
         <v>1192</v>
       </c>
@@ -15185,7 +15236,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="1196" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1196" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1196" s="1" t="s">
         <v>1193</v>
       </c>
@@ -15193,7 +15244,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="1197" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1197" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1197" s="1" t="s">
         <v>1194</v>
       </c>
@@ -15201,7 +15252,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="1198" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1198" spans="1:8" ht="30" x14ac:dyDescent="0.25">
       <c r="A1198" s="1" t="s">
         <v>1195</v>
       </c>
@@ -15209,7 +15260,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="1199" spans="1:2" ht="105" x14ac:dyDescent="0.25">
+    <row r="1199" spans="1:8" ht="105" x14ac:dyDescent="0.25">
       <c r="A1199" s="1" t="s">
         <v>1196</v>
       </c>
@@ -15217,7 +15268,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="1200" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1200" spans="1:8" ht="45" x14ac:dyDescent="0.25">
       <c r="A1200" s="1" t="s">
         <v>1197</v>
       </c>
@@ -18361,7 +18412,7 @@
   </sheetData>
   <autoFilter ref="A1:G1579" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1:B1579 A1585:B1048576">
+  <conditionalFormatting sqref="A1585:B1048576 A1:B1579">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
   <conditionalFormatting sqref="A1580:B1584">

</xml_diff>

<commit_message>
Hóa khoa quan lộc
</commit_message>
<xml_diff>
--- a/LuanHuynhDe.xlsx
+++ b/LuanHuynhDe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{473E174A-CD06-4FA2-A0C3-D37FE5871484}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{31DFF81F-E5FB-4211-9ECE-D068D785A3D5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="6346" uniqueCount="1752">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3181" uniqueCount="1758">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -5277,9 +5277,6 @@
     <t>Tình hình điều độ tiền bạc sẽ mỗi lúc càng ít đi, càng khó khăn hơn, việc phải lấy tiền đằng đông đắp vào đằng tây, xoay sở tiền cực nhọc</t>
   </si>
   <si>
-    <t>Là chủ về thế chất mạnh mẽ dẻo dai, có thể chịu đụng sự đả kích từ bên ngoài của Hóa Kị, thường thường còn có lực đề kháng đối với tai hại bất ngờ.</t>
-  </si>
-  <si>
     <t>Là chủ về thế chất mạnh mẽ dẻo dai, có thể chịu đụng sự đả kích từ bên ngoài của Hóa Kị, thường thường còn có lực đề kháng đối với tai hại bất ngờ. Cung vị khí số của cung tật ách cũng là cung dùng để tìm hiểu tâm tư sâu kín. Hóa Quyền ở cung huynh đệ, chủ về tâm tư sâu kín của mệnh tạo vận tác một cách mau lẹ, trong đó mệnh tạo còn có kì vọng tự lập tự cường, và ý đồ phấn đấu đi lên (nhưng những kì vọng và ý đồ của mệnh tạo sẽ khó thực hiện, vì Hóa Quyền ở "tha cung" nên sức tưởng tượng lớn hơn lực tạo tác).</t>
   </si>
   <si>
@@ -5287,6 +5284,27 @@
   </si>
   <si>
     <t>Cung huynh đệ là cung vị biểu hiện của cung điền trạch, có Hóa Quyền, thì đối với việc trang hoàng trong nhà mệnh tạo có yêu cầu thực dụng, có phong cách; hơn nữa, vì Hóa Quyền chủ về biến động lớn, nên gia cụ trong nhà hay thay đổi hoặc dời chuyển, và thường có khách đến thăm; vả lại, không loại trừ trường hợp chính bản thân mệnh tạo cũng thường hay dời chuyển.</t>
+  </si>
+  <si>
+    <t>Trường hợp Hóa Khoa ở cung huynh đệ, vì có lực tác động của tứ hóa khiến cung huynh đệ có biến động thay đổi, thông thường chủ về mệnh tạo không phải là con độc nhất, mà có anh chị em. Trường hợp Hóa Khoa ở cung huynh đệ, vì có tính so sánh nên phần nhiều anh chị em trông có khí chất và học vấn hơn mệnh tạo; thông thường họ có sở học tính chuyên, hay học lực cao hơn mệnh tạo. Hóa Khoa chủ về bảo vệ, trật tự hóa; trường hợp có Hóa Khoa ở cung huynh đệ là ngầm báo ông Trời che chở anh chị em của mệnh tạo, bảo vệ sinh mệnh hay tài sản của họ. Do có tác dụng trật tự hóa, làm cho thông suốt, hòa hợp, nên thường thường anh chị em rất thương yêu nhau; dù có xảy ra chuyện tranh chấp cãi vã với anh chị em, rốt cuộc vẫn có thể vãn hồi.</t>
+  </si>
+  <si>
+    <t>Cung huynh đệ còn có ý tượng là "kho tiền bạc", lúc xem xét ở góc độ "kho tiền bạc", đương nhiên yêu cầu cung này nên tĩnh, không nên động. Mà lực tác động của Hóa Khoa là "bảo vệ", "bảo đảm", nên trong trường hợp ở cung huynh đệ là chủ về lúc tuổi trẻ tiền túi và tiền để dành của mệnh tạo đã hơn người; ngoài ra, còn chủ về mệnh tạo quản lí tiền bạc khá cấn thận, hợp lí. Cung huynh đệ còn là cung vị đại biểu cho mẹ, trường hợp có Hóa Khoa, xét ở góc độ so sánh, mẹ là người thông tình đạt lí, xử lí việc nhà cũng có lớp lang rõ ràng. Cung huynh đệ còn là cầu nối giữa cung mệnh và cung phu thê, có thể dùng để xem về cha mẹ chồng hay cha mẹ vợ. Trường hợp có Hóa Khoa, thông thường song thân của "một nửa kia" là người thông tình đạt lí, không thù cựu, sẽ không làm khó mệnh tạo. Nhưng lực tác động của Hóa Khoa phần nhiều sẽ khiến cho bậc trưởng bối chi trợ lực cho mệnh tạo về tình cảm, chớ không phải về tiền bạc; lúc bậc trưởng bối giúp đỡ tiền bạc thì hầu hết đã là lúc mệnh tạo rất nguy cấp.</t>
+  </si>
+  <si>
+    <t>Cung huynh đệ là cung vị khí số của cung tật ách, trường hợp có Hóa Khoa, phần nhiều là chủ về mệnh tạo có sức khỏe tốt, thể chất không tệ, ít khi bị các bệnh vặt như cảm mạo.</t>
+  </si>
+  <si>
+    <t>Vì Hóa Khoa ở đối cung của cung nô bộc, nên sẽ khiến cho "nô bộc" của mệnh tạo ít có ý niệm bất chính trong đầu. Cũng do Hóa Khoa ở tuyến "huynh nô" là chủ về bảo vệ, giải ách, nên sẽ khiến mệnh tạo ít khi gặp bất trắc, vô cớ bị tốn hại, tổn thất.</t>
+  </si>
+  <si>
+    <t>Cung huynh đệ là cầu nối giữa mệnh tạo với vợ hoặc chồng, trường hợp có Hóa Khoa, có thể đoán là giữa hai người có trò chuyện trao đổi với nhau, cũng có không ít cơ hội kết giao bạn khác giới, mà còn có thể duy trì mối liên hệ vui vẻ. Hơn nữa, thường thường nhờ giữa vợ chồng có sự hiểu biết nhau, vì vậy dù không còn tình yêu, hai người vẫn có thể nói lời chia tay một cách tốt đẹp.</t>
+  </si>
+  <si>
+    <t>Cung huynh đệ còn là cung vị giao dịch của cung điền trạch, trường hợp có Hóa Khoa, lúc mệnh tạo muốn điều phối lại "điền trạch" của mình, thông thường đều có thể rời khỏi tay mình với giá cả hơp lí, mà không bị tổn thất. Bất động sản của mệnh tạo thường thường có vẻ bề ngoài thanh nhà, hoàn cảnh chung quanh không tệ; phần nhiều số bất động sản của mệnh tạo đều có thể giữ được nguyên giá trị, không bị ảnh hưởng lên xuống của thị trường.</t>
+  </si>
+  <si>
+    <t>Cung huynh đệ là "tha cung", có Hóa Khoa, chủ về bản thân mệnh tạo không có năng lực xử lí nguy cơ, mà thường thường đến gian đoạn thử hai mới được người khác trợ giúp, ít nhiêu mệnh tạo cũng có mặc cảm "bất túc". Hóa Khoa ở cung huynh đệ, là mệnh tạo giao cho anh chị em lực tác động của Khoa, nhưng không phải anh chị em là quý nhân của mệnh tạo, mà trái lại, mệnh tạo là quý nhân của anh chị em, sau khi trợ giúp và bảo vệ anh chị em rồi mệnh tạo mới có được cảnh anh em trợ giúp nhau.</t>
   </si>
 </sst>
 </file>
@@ -5641,10 +5659,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:H1584"/>
+  <dimension ref="A1:I1584"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1185" workbookViewId="0">
-      <selection activeCell="C1193" sqref="C1193"/>
+    <sheetView tabSelected="1" topLeftCell="D1194" workbookViewId="0">
+      <selection activeCell="J1194" sqref="J1194"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5656,6 +5674,7 @@
     <col min="6" max="6" width="39.42578125" customWidth="1"/>
     <col min="7" max="7" width="39.7109375" customWidth="1"/>
     <col min="8" max="8" width="23.7109375" customWidth="1"/>
+    <col min="9" max="9" width="43.42578125" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:2" x14ac:dyDescent="0.25">
@@ -10178,7 +10197,7 @@
         <v>595</v>
       </c>
     </row>
-    <row r="566" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="566" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A566" s="1" t="s">
         <v>596</v>
       </c>
@@ -13770,7 +13789,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="1015" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1015" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
         <v>1030</v>
       </c>
@@ -13994,7 +14013,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="1043" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1043" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1043" s="1" t="s">
         <v>1058</v>
       </c>
@@ -14106,7 +14125,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="1057" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1057" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1057" s="1" t="s">
         <v>1072</v>
       </c>
@@ -15130,7 +15149,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="1185" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1185" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1185" s="1" t="s">
         <v>1182</v>
       </c>
@@ -15138,7 +15157,7 @@
         <v>1631</v>
       </c>
     </row>
-    <row r="1186" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1186" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1186" s="1" t="s">
         <v>1183</v>
       </c>
@@ -15146,7 +15165,7 @@
         <v>1632</v>
       </c>
     </row>
-    <row r="1187" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1187" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1187" s="1" t="s">
         <v>1184</v>
       </c>
@@ -15154,7 +15173,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="1188" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1188" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1188" s="1" t="s">
         <v>1185</v>
       </c>
@@ -15162,7 +15181,7 @@
         <v>1633</v>
       </c>
     </row>
-    <row r="1189" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1189" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1189" s="1" t="s">
         <v>1186</v>
       </c>
@@ -15170,7 +15189,7 @@
         <v>1634</v>
       </c>
     </row>
-    <row r="1190" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1190" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1190" s="1" t="s">
         <v>1187</v>
       </c>
@@ -15178,7 +15197,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="1191" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1191" s="1" t="s">
         <v>1188</v>
       </c>
@@ -15186,7 +15205,7 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="1192" spans="1:8" ht="60" x14ac:dyDescent="0.25">
+    <row r="1192" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1192" s="1" t="s">
         <v>1189</v>
       </c>
@@ -15194,7 +15213,7 @@
         <v>1636</v>
       </c>
     </row>
-    <row r="1193" spans="1:8" ht="315" x14ac:dyDescent="0.25">
+    <row r="1193" spans="1:9" ht="315" x14ac:dyDescent="0.25">
       <c r="A1193" s="1" t="s">
         <v>1190</v>
       </c>
@@ -15211,24 +15230,45 @@
         <v>1745</v>
       </c>
       <c r="F1193" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="G1193" s="1" t="s">
         <v>1749</v>
       </c>
-      <c r="G1193" s="1" t="s">
+      <c r="H1193" s="1" t="s">
         <v>1750</v>
       </c>
-      <c r="H1193" s="1" t="s">
-        <v>1751</v>
-      </c>
-    </row>
-    <row r="1194" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1194" spans="1:9" ht="300" x14ac:dyDescent="0.25">
       <c r="A1194" s="1" t="s">
         <v>1191</v>
       </c>
       <c r="B1194" s="1" t="s">
         <v>1639</v>
       </c>
-    </row>
-    <row r="1195" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+      <c r="C1194" s="1" t="s">
+        <v>1751</v>
+      </c>
+      <c r="D1194" s="1" t="s">
+        <v>1752</v>
+      </c>
+      <c r="E1194" s="1" t="s">
+        <v>1753</v>
+      </c>
+      <c r="F1194" s="1" t="s">
+        <v>1754</v>
+      </c>
+      <c r="G1194" s="1" t="s">
+        <v>1755</v>
+      </c>
+      <c r="H1194" s="1" t="s">
+        <v>1756</v>
+      </c>
+      <c r="I1194" s="1" t="s">
+        <v>1757</v>
+      </c>
+    </row>
+    <row r="1195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1195" s="1" t="s">
         <v>1192</v>
       </c>
@@ -15236,7 +15276,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="1196" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1196" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1196" s="1" t="s">
         <v>1193</v>
       </c>
@@ -15244,7 +15284,7 @@
         <v>1641</v>
       </c>
     </row>
-    <row r="1197" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1197" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1197" s="1" t="s">
         <v>1194</v>
       </c>
@@ -15252,7 +15292,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="1198" spans="1:8" ht="30" x14ac:dyDescent="0.25">
+    <row r="1198" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1198" s="1" t="s">
         <v>1195</v>
       </c>
@@ -15260,7 +15300,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="1199" spans="1:8" ht="105" x14ac:dyDescent="0.25">
+    <row r="1199" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A1199" s="1" t="s">
         <v>1196</v>
       </c>
@@ -15268,7 +15308,7 @@
         <v>1644</v>
       </c>
     </row>
-    <row r="1200" spans="1:8" ht="45" x14ac:dyDescent="0.25">
+    <row r="1200" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1200" s="1" t="s">
         <v>1197</v>
       </c>

</xml_diff>

<commit_message>
Fix bug version 3
</commit_message>
<xml_diff>
--- a/LuanHuynhDe.xlsx
+++ b/LuanHuynhDe.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Tuvi\TuVi\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D843BFC5-7D18-4990-B13C-BB479924E72F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{87093E91-B806-40AF-ADC3-CA7E23402B14}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -16,7 +16,7 @@
     <sheet name="Sheet2" sheetId="2" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$G$1579</definedName>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet2!$A$1:$G$1578</definedName>
   </definedNames>
   <calcPr calcId="181029"/>
   <extLst>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3189" uniqueCount="1766">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3187" uniqueCount="1765">
   <si>
     <t>Vũ Khúc và Tham Lang đồng cung tại Mùi</t>
   </si>
@@ -2284,9 +2284,6 @@
   </si>
   <si>
     <t>Hoá Khoa toạ thủ cung Huynh Đệ gặp Tử Vi, Thiên Phủ</t>
-  </si>
-  <si>
-    <t>Hóa Kỵ toạ thủ cung Huynh Đệ</t>
   </si>
   <si>
     <t>Hóa Kỵ toạ thủ cung Huynh Đệ gặp Hỏa Tinh, Linh Tinh, Kình Dương, Đà La</t>
@@ -5683,10 +5680,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}">
-  <dimension ref="A1:J1584"/>
+  <dimension ref="A1:J1583"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A1156" workbookViewId="0">
-      <selection activeCell="C1161" sqref="C1161"/>
+    <sheetView tabSelected="1" topLeftCell="A722" workbookViewId="0">
+      <selection activeCell="A744" sqref="A744"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -5707,7 +5704,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="1" t="s">
-        <v>1698</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="2" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -5715,7 +5712,7 @@
         <v>40</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>1600</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -5723,7 +5720,7 @@
         <v>41</v>
       </c>
       <c r="B3" s="1" t="s">
-        <v>1601</v>
+        <v>1600</v>
       </c>
     </row>
     <row r="4" spans="1:2" ht="60" x14ac:dyDescent="0.25">
@@ -5731,7 +5728,7 @@
         <v>42</v>
       </c>
       <c r="B4" s="1" t="s">
-        <v>1602</v>
+        <v>1601</v>
       </c>
     </row>
     <row r="5" spans="1:2" x14ac:dyDescent="0.25">
@@ -5739,7 +5736,7 @@
         <v>43</v>
       </c>
       <c r="B5" s="1" t="s">
-        <v>1603</v>
+        <v>1602</v>
       </c>
     </row>
     <row r="6" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -5747,7 +5744,7 @@
         <v>44</v>
       </c>
       <c r="B6" s="1" t="s">
-        <v>1604</v>
+        <v>1603</v>
       </c>
     </row>
     <row r="7" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -5755,7 +5752,7 @@
         <v>45</v>
       </c>
       <c r="B7" s="1" t="s">
-        <v>1605</v>
+        <v>1604</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -5779,7 +5776,7 @@
         <v>48</v>
       </c>
       <c r="B10" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="11" spans="1:2" x14ac:dyDescent="0.25">
@@ -5971,7 +5968,7 @@
         <v>70</v>
       </c>
       <c r="B34" t="s">
-        <v>1565</v>
+        <v>1564</v>
       </c>
     </row>
     <row r="35" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -6019,7 +6016,7 @@
         <v>76</v>
       </c>
       <c r="B40" s="1" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="41" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -6067,7 +6064,7 @@
         <v>82</v>
       </c>
       <c r="B46" s="1" t="s">
-        <v>1564</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="47" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -11387,7 +11384,7 @@
         <v>741</v>
       </c>
       <c r="B711" s="1" t="s">
-        <v>1746</v>
+        <v>1745</v>
       </c>
     </row>
     <row r="712" spans="1:2" x14ac:dyDescent="0.25">
@@ -11411,7 +11408,7 @@
         <v>744</v>
       </c>
       <c r="B714" s="1" t="s">
-        <v>1747</v>
+        <v>1746</v>
       </c>
     </row>
     <row r="715" spans="1:2" x14ac:dyDescent="0.25">
@@ -11534,7 +11531,7 @@
         <v>759</v>
       </c>
     </row>
-    <row r="730" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="730" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A730" s="1" t="s">
         <v>760</v>
       </c>
@@ -11542,7 +11539,7 @@
         <v>760</v>
       </c>
     </row>
-    <row r="731" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="731" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A731" s="1" t="s">
         <v>761</v>
       </c>
@@ -11702,7 +11699,7 @@
         <v>780</v>
       </c>
     </row>
-    <row r="751" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="751" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A751" s="1" t="s">
         <v>781</v>
       </c>
@@ -11710,7 +11707,7 @@
         <v>781</v>
       </c>
     </row>
-    <row r="752" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="752" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A752" s="1" t="s">
         <v>782</v>
       </c>
@@ -11726,7 +11723,7 @@
         <v>783</v>
       </c>
     </row>
-    <row r="754" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="754" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A754" s="1" t="s">
         <v>784</v>
       </c>
@@ -11734,7 +11731,7 @@
         <v>784</v>
       </c>
     </row>
-    <row r="755" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="755" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A755" s="1" t="s">
         <v>785</v>
       </c>
@@ -11918,7 +11915,7 @@
         <v>807</v>
       </c>
     </row>
-    <row r="778" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="778" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A778" s="1" t="s">
         <v>808</v>
       </c>
@@ -11926,7 +11923,7 @@
         <v>808</v>
       </c>
     </row>
-    <row r="779" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="779" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A779" s="1" t="s">
         <v>809</v>
       </c>
@@ -11950,7 +11947,7 @@
         <v>811</v>
       </c>
     </row>
-    <row r="782" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="782" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A782" s="1" t="s">
         <v>812</v>
       </c>
@@ -11958,7 +11955,7 @@
         <v>812</v>
       </c>
     </row>
-    <row r="783" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="783" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A783" s="1" t="s">
         <v>813</v>
       </c>
@@ -12070,7 +12067,7 @@
         <v>826</v>
       </c>
     </row>
-    <row r="797" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="797" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A797" s="1" t="s">
         <v>827</v>
       </c>
@@ -12078,7 +12075,7 @@
         <v>827</v>
       </c>
     </row>
-    <row r="798" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="798" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A798" s="1" t="s">
         <v>828</v>
       </c>
@@ -12086,7 +12083,7 @@
         <v>828</v>
       </c>
     </row>
-    <row r="799" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="799" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A799" s="1" t="s">
         <v>829</v>
       </c>
@@ -12094,7 +12091,7 @@
         <v>829</v>
       </c>
     </row>
-    <row r="800" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="800" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A800" s="1" t="s">
         <v>830</v>
       </c>
@@ -12102,7 +12099,7 @@
         <v>830</v>
       </c>
     </row>
-    <row r="801" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="801" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A801" s="1" t="s">
         <v>831</v>
       </c>
@@ -12110,7 +12107,7 @@
         <v>831</v>
       </c>
     </row>
-    <row r="802" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="802" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A802" s="1" t="s">
         <v>832</v>
       </c>
@@ -12118,7 +12115,7 @@
         <v>832</v>
       </c>
     </row>
-    <row r="803" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="803" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A803" s="1" t="s">
         <v>833</v>
       </c>
@@ -12126,7 +12123,7 @@
         <v>833</v>
       </c>
     </row>
-    <row r="804" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="804" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A804" s="1" t="s">
         <v>834</v>
       </c>
@@ -12238,7 +12235,7 @@
         <v>847</v>
       </c>
     </row>
-    <row r="818" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="818" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A818" s="1" t="s">
         <v>848</v>
       </c>
@@ -12254,7 +12251,7 @@
         <v>849</v>
       </c>
     </row>
-    <row r="820" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="820" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A820" s="1" t="s">
         <v>850</v>
       </c>
@@ -12270,7 +12267,7 @@
         <v>851</v>
       </c>
     </row>
-    <row r="822" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="822" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A822" s="1" t="s">
         <v>852</v>
       </c>
@@ -12286,7 +12283,7 @@
         <v>853</v>
       </c>
     </row>
-    <row r="824" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="824" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A824" s="1" t="s">
         <v>854</v>
       </c>
@@ -12302,7 +12299,7 @@
         <v>855</v>
       </c>
     </row>
-    <row r="826" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="826" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A826" s="1" t="s">
         <v>856</v>
       </c>
@@ -12318,7 +12315,7 @@
         <v>857</v>
       </c>
     </row>
-    <row r="828" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="828" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A828" s="1" t="s">
         <v>858</v>
       </c>
@@ -12334,7 +12331,7 @@
         <v>859</v>
       </c>
     </row>
-    <row r="830" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="830" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A830" s="1" t="s">
         <v>860</v>
       </c>
@@ -12366,7 +12363,7 @@
         <v>863</v>
       </c>
     </row>
-    <row r="834" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="834" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A834" s="1" t="s">
         <v>864</v>
       </c>
@@ -12374,7 +12371,7 @@
         <v>864</v>
       </c>
     </row>
-    <row r="835" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="835" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A835" s="1" t="s">
         <v>865</v>
       </c>
@@ -12398,7 +12395,7 @@
         <v>867</v>
       </c>
     </row>
-    <row r="838" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="838" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A838" s="1" t="s">
         <v>868</v>
       </c>
@@ -12408,146 +12405,146 @@
     </row>
     <row r="839" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A839" s="1" t="s">
-        <v>869</v>
+        <v>7</v>
       </c>
       <c r="B839" s="1" t="s">
-        <v>869</v>
+        <v>7</v>
       </c>
     </row>
     <row r="840" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A840" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B840" s="1" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
     </row>
     <row r="841" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A841" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
       <c r="B841" s="1" t="s">
-        <v>8</v>
+        <v>9</v>
       </c>
     </row>
     <row r="842" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A842" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
       <c r="B842" s="1" t="s">
-        <v>9</v>
+        <v>10</v>
       </c>
     </row>
     <row r="843" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A843" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
       <c r="B843" s="1" t="s">
-        <v>10</v>
+        <v>11</v>
       </c>
     </row>
     <row r="844" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A844" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
       <c r="B844" s="1" t="s">
-        <v>11</v>
+        <v>12</v>
       </c>
     </row>
     <row r="845" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A845" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
       <c r="B845" s="1" t="s">
-        <v>12</v>
+        <v>13</v>
       </c>
     </row>
     <row r="846" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A846" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B846" s="1" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
     </row>
     <row r="847" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A847" s="1" t="s">
-        <v>14</v>
+        <v>869</v>
       </c>
       <c r="B847" s="1" t="s">
-        <v>14</v>
+        <v>869</v>
       </c>
     </row>
     <row r="848" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A848" s="1" t="s">
-        <v>870</v>
+        <v>15</v>
       </c>
       <c r="B848" s="1" t="s">
-        <v>870</v>
+        <v>15</v>
       </c>
     </row>
     <row r="849" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A849" s="1" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
       <c r="B849" s="1" t="s">
-        <v>15</v>
-      </c>
-    </row>
-    <row r="850" spans="1:2" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="850" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A850" s="1" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B850" s="1" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="851" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="851" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A851" s="1" t="s">
-        <v>17</v>
+        <v>870</v>
       </c>
       <c r="B851" s="1" t="s">
-        <v>17</v>
+        <v>870</v>
       </c>
     </row>
     <row r="852" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A852" s="1" t="s">
-        <v>871</v>
+        <v>18</v>
       </c>
       <c r="B852" s="1" t="s">
-        <v>871</v>
-      </c>
-    </row>
-    <row r="853" spans="1:2" x14ac:dyDescent="0.25">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="853" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A853" s="1" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B853" s="1" t="s">
-        <v>18</v>
-      </c>
-    </row>
-    <row r="854" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="854" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A854" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="B854" s="1" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
     </row>
     <row r="855" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A855" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
       <c r="B855" s="1" t="s">
-        <v>20</v>
+        <v>21</v>
       </c>
     </row>
     <row r="856" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A856" s="1" t="s">
-        <v>21</v>
+        <v>871</v>
       </c>
       <c r="B856" s="1" t="s">
-        <v>21</v>
+        <v>871</v>
       </c>
     </row>
     <row r="857" spans="1:2" x14ac:dyDescent="0.25">
@@ -12590,7 +12587,7 @@
         <v>876</v>
       </c>
     </row>
-    <row r="862" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="862" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A862" s="1" t="s">
         <v>877</v>
       </c>
@@ -12614,7 +12611,7 @@
         <v>879</v>
       </c>
     </row>
-    <row r="865" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="865" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A865" s="1" t="s">
         <v>880</v>
       </c>
@@ -12622,7 +12619,7 @@
         <v>880</v>
       </c>
     </row>
-    <row r="866" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="866" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A866" s="1" t="s">
         <v>881</v>
       </c>
@@ -12646,7 +12643,7 @@
         <v>883</v>
       </c>
     </row>
-    <row r="869" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="869" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A869" s="1" t="s">
         <v>884</v>
       </c>
@@ -12654,7 +12651,7 @@
         <v>884</v>
       </c>
     </row>
-    <row r="870" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="870" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A870" s="1" t="s">
         <v>885</v>
       </c>
@@ -12662,7 +12659,7 @@
         <v>885</v>
       </c>
     </row>
-    <row r="871" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="871" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A871" s="1" t="s">
         <v>886</v>
       </c>
@@ -12686,7 +12683,7 @@
         <v>888</v>
       </c>
     </row>
-    <row r="874" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="874" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A874" s="1" t="s">
         <v>889</v>
       </c>
@@ -12694,7 +12691,7 @@
         <v>889</v>
       </c>
     </row>
-    <row r="875" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="875" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A875" s="1" t="s">
         <v>890</v>
       </c>
@@ -12702,7 +12699,7 @@
         <v>890</v>
       </c>
     </row>
-    <row r="876" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="876" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A876" s="1" t="s">
         <v>891</v>
       </c>
@@ -12726,7 +12723,7 @@
         <v>893</v>
       </c>
     </row>
-    <row r="879" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="879" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A879" s="1" t="s">
         <v>894</v>
       </c>
@@ -12734,7 +12731,7 @@
         <v>894</v>
       </c>
     </row>
-    <row r="880" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="880" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A880" s="1" t="s">
         <v>895</v>
       </c>
@@ -12742,7 +12739,7 @@
         <v>895</v>
       </c>
     </row>
-    <row r="881" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="881" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A881" s="1" t="s">
         <v>896</v>
       </c>
@@ -12750,7 +12747,7 @@
         <v>896</v>
       </c>
     </row>
-    <row r="882" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="882" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A882" s="1" t="s">
         <v>897</v>
       </c>
@@ -12790,7 +12787,7 @@
         <v>901</v>
       </c>
     </row>
-    <row r="887" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="887" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A887" s="1" t="s">
         <v>902</v>
       </c>
@@ -12798,7 +12795,7 @@
         <v>902</v>
       </c>
     </row>
-    <row r="888" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="888" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A888" s="1" t="s">
         <v>903</v>
       </c>
@@ -12838,7 +12835,7 @@
         <v>907</v>
       </c>
     </row>
-    <row r="893" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="893" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A893" s="1" t="s">
         <v>908</v>
       </c>
@@ -12846,7 +12843,7 @@
         <v>908</v>
       </c>
     </row>
-    <row r="894" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="894" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A894" s="1" t="s">
         <v>909</v>
       </c>
@@ -12886,7 +12883,7 @@
         <v>913</v>
       </c>
     </row>
-    <row r="899" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="899" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A899" s="1" t="s">
         <v>914</v>
       </c>
@@ -12894,7 +12891,7 @@
         <v>914</v>
       </c>
     </row>
-    <row r="900" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="900" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A900" s="1" t="s">
         <v>915</v>
       </c>
@@ -12934,7 +12931,7 @@
         <v>919</v>
       </c>
     </row>
-    <row r="905" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="905" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A905" s="1" t="s">
         <v>920</v>
       </c>
@@ -12974,7 +12971,7 @@
         <v>924</v>
       </c>
     </row>
-    <row r="910" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="910" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A910" s="1" t="s">
         <v>925</v>
       </c>
@@ -12990,7 +12987,7 @@
         <v>926</v>
       </c>
     </row>
-    <row r="912" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="912" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A912" s="1" t="s">
         <v>927</v>
       </c>
@@ -13014,7 +13011,7 @@
         <v>929</v>
       </c>
     </row>
-    <row r="915" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="915" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A915" s="1" t="s">
         <v>930</v>
       </c>
@@ -13038,7 +13035,7 @@
         <v>932</v>
       </c>
     </row>
-    <row r="918" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="918" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A918" s="1" t="s">
         <v>933</v>
       </c>
@@ -13062,7 +13059,7 @@
         <v>935</v>
       </c>
     </row>
-    <row r="921" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="921" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A921" s="1" t="s">
         <v>936</v>
       </c>
@@ -13110,7 +13107,7 @@
         <v>941</v>
       </c>
     </row>
-    <row r="927" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="927" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A927" s="1" t="s">
         <v>942</v>
       </c>
@@ -13134,7 +13131,7 @@
         <v>944</v>
       </c>
     </row>
-    <row r="930" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="930" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A930" s="1" t="s">
         <v>945</v>
       </c>
@@ -13166,7 +13163,7 @@
         <v>948</v>
       </c>
     </row>
-    <row r="934" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="934" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A934" s="1" t="s">
         <v>949</v>
       </c>
@@ -13214,7 +13211,7 @@
         <v>954</v>
       </c>
     </row>
-    <row r="940" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="940" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A940" s="1" t="s">
         <v>955</v>
       </c>
@@ -13222,7 +13219,7 @@
         <v>955</v>
       </c>
     </row>
-    <row r="941" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="941" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A941" s="1" t="s">
         <v>956</v>
       </c>
@@ -13286,7 +13283,7 @@
         <v>963</v>
       </c>
     </row>
-    <row r="949" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="949" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A949" s="1" t="s">
         <v>964</v>
       </c>
@@ -13302,7 +13299,7 @@
         <v>965</v>
       </c>
     </row>
-    <row r="951" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="951" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A951" s="1" t="s">
         <v>966</v>
       </c>
@@ -13310,7 +13307,7 @@
         <v>966</v>
       </c>
     </row>
-    <row r="952" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="952" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A952" s="1" t="s">
         <v>967</v>
       </c>
@@ -13326,7 +13323,7 @@
         <v>968</v>
       </c>
     </row>
-    <row r="954" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="954" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A954" s="1" t="s">
         <v>969</v>
       </c>
@@ -13406,7 +13403,7 @@
         <v>978</v>
       </c>
     </row>
-    <row r="964" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="964" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A964" s="1" t="s">
         <v>979</v>
       </c>
@@ -13414,7 +13411,7 @@
         <v>979</v>
       </c>
     </row>
-    <row r="965" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="965" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A965" s="1" t="s">
         <v>980</v>
       </c>
@@ -13438,7 +13435,7 @@
         <v>982</v>
       </c>
     </row>
-    <row r="968" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="968" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A968" s="1" t="s">
         <v>983</v>
       </c>
@@ -13446,7 +13443,7 @@
         <v>983</v>
       </c>
     </row>
-    <row r="969" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="969" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A969" s="1" t="s">
         <v>984</v>
       </c>
@@ -13486,7 +13483,7 @@
         <v>988</v>
       </c>
     </row>
-    <row r="974" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="974" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A974" s="1" t="s">
         <v>989</v>
       </c>
@@ -13494,7 +13491,7 @@
         <v>989</v>
       </c>
     </row>
-    <row r="975" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="975" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A975" s="1" t="s">
         <v>990</v>
       </c>
@@ -13502,7 +13499,7 @@
         <v>990</v>
       </c>
     </row>
-    <row r="976" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="976" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A976" s="1" t="s">
         <v>991</v>
       </c>
@@ -13518,7 +13515,7 @@
         <v>992</v>
       </c>
     </row>
-    <row r="978" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="978" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A978" s="1" t="s">
         <v>993</v>
       </c>
@@ -13526,7 +13523,7 @@
         <v>993</v>
       </c>
     </row>
-    <row r="979" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="979" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A979" s="1" t="s">
         <v>994</v>
       </c>
@@ -13534,7 +13531,7 @@
         <v>994</v>
       </c>
     </row>
-    <row r="980" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="980" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A980" s="1" t="s">
         <v>995</v>
       </c>
@@ -13550,7 +13547,7 @@
         <v>996</v>
       </c>
     </row>
-    <row r="982" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="982" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A982" s="1" t="s">
         <v>997</v>
       </c>
@@ -13558,7 +13555,7 @@
         <v>997</v>
       </c>
     </row>
-    <row r="983" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="983" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A983" s="1" t="s">
         <v>998</v>
       </c>
@@ -13566,7 +13563,7 @@
         <v>998</v>
       </c>
     </row>
-    <row r="984" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="984" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A984" s="1" t="s">
         <v>999</v>
       </c>
@@ -13582,7 +13579,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="986" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="986" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A986" s="1" t="s">
         <v>1001</v>
       </c>
@@ -13590,7 +13587,7 @@
         <v>1001</v>
       </c>
     </row>
-    <row r="987" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="987" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A987" s="1" t="s">
         <v>1002</v>
       </c>
@@ -13598,7 +13595,7 @@
         <v>1002</v>
       </c>
     </row>
-    <row r="988" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="988" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A988" s="1" t="s">
         <v>1003</v>
       </c>
@@ -13614,7 +13611,7 @@
         <v>1004</v>
       </c>
     </row>
-    <row r="990" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="990" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A990" s="1" t="s">
         <v>1005</v>
       </c>
@@ -13622,7 +13619,7 @@
         <v>1005</v>
       </c>
     </row>
-    <row r="991" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="991" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A991" s="1" t="s">
         <v>1006</v>
       </c>
@@ -13638,7 +13635,7 @@
         <v>1007</v>
       </c>
     </row>
-    <row r="993" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="993" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A993" s="1" t="s">
         <v>1008</v>
       </c>
@@ -13646,7 +13643,7 @@
         <v>1008</v>
       </c>
     </row>
-    <row r="994" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="994" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A994" s="1" t="s">
         <v>1009</v>
       </c>
@@ -13662,7 +13659,7 @@
         <v>1010</v>
       </c>
     </row>
-    <row r="996" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="996" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A996" s="1" t="s">
         <v>1011</v>
       </c>
@@ -13670,7 +13667,7 @@
         <v>1011</v>
       </c>
     </row>
-    <row r="997" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="997" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A997" s="1" t="s">
         <v>1012</v>
       </c>
@@ -13686,7 +13683,7 @@
         <v>1013</v>
       </c>
     </row>
-    <row r="999" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="999" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A999" s="1" t="s">
         <v>1014</v>
       </c>
@@ -13694,7 +13691,7 @@
         <v>1014</v>
       </c>
     </row>
-    <row r="1000" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1000" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1000" s="1" t="s">
         <v>1015</v>
       </c>
@@ -13710,7 +13707,7 @@
         <v>1016</v>
       </c>
     </row>
-    <row r="1002" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1002" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1002" s="1" t="s">
         <v>1017</v>
       </c>
@@ -13718,7 +13715,7 @@
         <v>1017</v>
       </c>
     </row>
-    <row r="1003" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1003" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1003" s="1" t="s">
         <v>1018</v>
       </c>
@@ -13742,7 +13739,7 @@
         <v>1020</v>
       </c>
     </row>
-    <row r="1006" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1006" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1006" s="1" t="s">
         <v>1021</v>
       </c>
@@ -13806,7 +13803,7 @@
         <v>1028</v>
       </c>
     </row>
-    <row r="1014" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1014" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1014" s="1" t="s">
         <v>1029</v>
       </c>
@@ -13814,7 +13811,7 @@
         <v>1029</v>
       </c>
     </row>
-    <row r="1015" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1015" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1015" s="1" t="s">
         <v>1030</v>
       </c>
@@ -13862,7 +13859,7 @@
         <v>1035</v>
       </c>
     </row>
-    <row r="1021" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1021" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1021" s="1" t="s">
         <v>1036</v>
       </c>
@@ -13870,7 +13867,7 @@
         <v>1036</v>
       </c>
     </row>
-    <row r="1022" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1022" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1022" s="1" t="s">
         <v>1037</v>
       </c>
@@ -13918,7 +13915,7 @@
         <v>1042</v>
       </c>
     </row>
-    <row r="1028" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1028" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1028" s="1" t="s">
         <v>1043</v>
       </c>
@@ -13926,7 +13923,7 @@
         <v>1043</v>
       </c>
     </row>
-    <row r="1029" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1029" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1029" s="1" t="s">
         <v>1044</v>
       </c>
@@ -13974,7 +13971,7 @@
         <v>1049</v>
       </c>
     </row>
-    <row r="1035" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1035" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1035" s="1" t="s">
         <v>1050</v>
       </c>
@@ -13982,7 +13979,7 @@
         <v>1050</v>
       </c>
     </row>
-    <row r="1036" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1036" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1036" s="1" t="s">
         <v>1051</v>
       </c>
@@ -14030,7 +14027,7 @@
         <v>1056</v>
       </c>
     </row>
-    <row r="1042" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1042" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1042" s="1" t="s">
         <v>1057</v>
       </c>
@@ -14038,7 +14035,7 @@
         <v>1057</v>
       </c>
     </row>
-    <row r="1043" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1043" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1043" s="1" t="s">
         <v>1058</v>
       </c>
@@ -14086,7 +14083,7 @@
         <v>1063</v>
       </c>
     </row>
-    <row r="1049" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1049" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1049" s="1" t="s">
         <v>1064</v>
       </c>
@@ -14094,7 +14091,7 @@
         <v>1064</v>
       </c>
     </row>
-    <row r="1050" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1050" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1050" s="1" t="s">
         <v>1065</v>
       </c>
@@ -14142,7 +14139,7 @@
         <v>1070</v>
       </c>
     </row>
-    <row r="1056" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1056" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1056" s="1" t="s">
         <v>1071</v>
       </c>
@@ -14150,7 +14147,7 @@
         <v>1071</v>
       </c>
     </row>
-    <row r="1057" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1057" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1057" s="1" t="s">
         <v>1072</v>
       </c>
@@ -14198,7 +14195,7 @@
         <v>1077</v>
       </c>
     </row>
-    <row r="1063" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1063" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1063" s="1" t="s">
         <v>1078</v>
       </c>
@@ -14206,7 +14203,7 @@
         <v>1078</v>
       </c>
     </row>
-    <row r="1064" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1064" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1064" s="1" t="s">
         <v>1079</v>
       </c>
@@ -14254,7 +14251,7 @@
         <v>1084</v>
       </c>
     </row>
-    <row r="1070" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1070" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1070" s="1" t="s">
         <v>1085</v>
       </c>
@@ -14262,7 +14259,7 @@
         <v>1085</v>
       </c>
     </row>
-    <row r="1071" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1071" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1071" s="1" t="s">
         <v>1086</v>
       </c>
@@ -14310,7 +14307,7 @@
         <v>1091</v>
       </c>
     </row>
-    <row r="1077" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1077" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1077" s="1" t="s">
         <v>1092</v>
       </c>
@@ -14318,7 +14315,7 @@
         <v>1092</v>
       </c>
     </row>
-    <row r="1078" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1078" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1078" s="1" t="s">
         <v>1093</v>
       </c>
@@ -14366,7 +14363,7 @@
         <v>1098</v>
       </c>
     </row>
-    <row r="1084" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1084" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1084" s="1" t="s">
         <v>1099</v>
       </c>
@@ -14374,7 +14371,7 @@
         <v>1099</v>
       </c>
     </row>
-    <row r="1085" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1085" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1085" s="1" t="s">
         <v>1100</v>
       </c>
@@ -14422,7 +14419,7 @@
         <v>1105</v>
       </c>
     </row>
-    <row r="1091" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1091" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1091" s="1" t="s">
         <v>1106</v>
       </c>
@@ -14430,7 +14427,7 @@
         <v>1106</v>
       </c>
     </row>
-    <row r="1092" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1092" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1092" s="1" t="s">
         <v>1107</v>
       </c>
@@ -14574,7 +14571,7 @@
         <v>1124</v>
       </c>
     </row>
-    <row r="1110" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1110" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1110" s="1" t="s">
         <v>1125</v>
       </c>
@@ -14590,7 +14587,7 @@
         <v>1126</v>
       </c>
     </row>
-    <row r="1112" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1112" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1112" s="1" t="s">
         <v>1127</v>
       </c>
@@ -14598,7 +14595,7 @@
         <v>1127</v>
       </c>
     </row>
-    <row r="1113" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1113" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1113" s="1" t="s">
         <v>1128</v>
       </c>
@@ -14606,7 +14603,7 @@
         <v>1128</v>
       </c>
     </row>
-    <row r="1114" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1114" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1114" s="1" t="s">
         <v>1129</v>
       </c>
@@ -14638,7 +14635,7 @@
         <v>1132</v>
       </c>
     </row>
-    <row r="1118" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1118" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1118" s="1" t="s">
         <v>1133</v>
       </c>
@@ -14654,7 +14651,7 @@
         <v>1134</v>
       </c>
     </row>
-    <row r="1120" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1120" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1120" s="1" t="s">
         <v>1135</v>
       </c>
@@ -14662,7 +14659,7 @@
         <v>1135</v>
       </c>
     </row>
-    <row r="1121" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1121" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1121" s="1" t="s">
         <v>1136</v>
       </c>
@@ -14670,7 +14667,7 @@
         <v>1136</v>
       </c>
     </row>
-    <row r="1122" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1122" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1122" s="1" t="s">
         <v>1137</v>
       </c>
@@ -14726,7 +14723,7 @@
         <v>1143</v>
       </c>
     </row>
-    <row r="1129" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1129" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1129" s="1" t="s">
         <v>1144</v>
       </c>
@@ -14742,7 +14739,7 @@
         <v>1145</v>
       </c>
     </row>
-    <row r="1131" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1131" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1131" s="1" t="s">
         <v>1146</v>
       </c>
@@ -14790,7 +14787,7 @@
         <v>1151</v>
       </c>
     </row>
-    <row r="1137" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1137" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1137" s="1" t="s">
         <v>1152</v>
       </c>
@@ -14798,7 +14795,7 @@
         <v>1152</v>
       </c>
     </row>
-    <row r="1138" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1138" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1138" s="1" t="s">
         <v>1153</v>
       </c>
@@ -14822,7 +14819,7 @@
         <v>1155</v>
       </c>
     </row>
-    <row r="1141" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1141" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1141" s="1" t="s">
         <v>1156</v>
       </c>
@@ -14830,7 +14827,7 @@
         <v>1156</v>
       </c>
     </row>
-    <row r="1142" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1142" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1142" s="1" t="s">
         <v>1157</v>
       </c>
@@ -14846,7 +14843,7 @@
         <v>1158</v>
       </c>
     </row>
-    <row r="1144" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1144" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1144" s="1" t="s">
         <v>1159</v>
       </c>
@@ -14854,7 +14851,7 @@
         <v>1159</v>
       </c>
     </row>
-    <row r="1145" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1145" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1145" s="1" t="s">
         <v>1160</v>
       </c>
@@ -14870,97 +14867,97 @@
         <v>1161</v>
       </c>
     </row>
-    <row r="1147" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1147" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1147" s="1" t="s">
-        <v>1162</v>
+        <v>22</v>
       </c>
       <c r="B1147" s="1" t="s">
-        <v>1162</v>
-      </c>
-    </row>
-    <row r="1148" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1700</v>
+      </c>
+    </row>
+    <row r="1148" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1148" s="1" t="s">
-        <v>22</v>
+        <v>23</v>
       </c>
       <c r="B1148" s="1" t="s">
-        <v>1701</v>
+        <v>1723</v>
       </c>
     </row>
     <row r="1149" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1149" s="1" t="s">
-        <v>23</v>
+        <v>24</v>
       </c>
       <c r="B1149" s="1" t="s">
-        <v>1724</v>
+        <v>1711</v>
       </c>
     </row>
     <row r="1150" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1150" s="1" t="s">
-        <v>24</v>
+        <v>25</v>
       </c>
       <c r="B1150" s="1" t="s">
-        <v>1712</v>
+        <v>1686</v>
       </c>
     </row>
     <row r="1151" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1151" s="1" t="s">
-        <v>25</v>
+        <v>26</v>
       </c>
       <c r="B1151" s="1" t="s">
-        <v>1687</v>
+        <v>26</v>
       </c>
     </row>
     <row r="1152" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1152" s="1" t="s">
-        <v>26</v>
+        <v>27</v>
       </c>
       <c r="B1152" s="1" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="1153" spans="1:10" x14ac:dyDescent="0.25">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="1153" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1153" s="1" t="s">
-        <v>27</v>
+        <v>28</v>
       </c>
       <c r="B1153" s="1" t="s">
         <v>1606</v>
       </c>
     </row>
-    <row r="1154" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1154" spans="1:10" ht="75" x14ac:dyDescent="0.25">
       <c r="A1154" s="1" t="s">
-        <v>28</v>
+        <v>29</v>
       </c>
       <c r="B1154" s="1" t="s">
         <v>1607</v>
       </c>
     </row>
-    <row r="1155" spans="1:10" ht="75" x14ac:dyDescent="0.25">
+    <row r="1155" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1155" s="1" t="s">
-        <v>29</v>
+        <v>30</v>
       </c>
       <c r="B1155" s="1" t="s">
         <v>1608</v>
       </c>
     </row>
-    <row r="1156" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1156" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1156" s="1" t="s">
-        <v>30</v>
+        <v>31</v>
       </c>
       <c r="B1156" s="1" t="s">
         <v>1609</v>
       </c>
     </row>
-    <row r="1157" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    <row r="1157" spans="1:10" ht="105" x14ac:dyDescent="0.25">
       <c r="A1157" s="1" t="s">
-        <v>31</v>
+        <v>32</v>
       </c>
       <c r="B1157" s="1" t="s">
         <v>1610</v>
       </c>
     </row>
-    <row r="1158" spans="1:10" ht="105" x14ac:dyDescent="0.25">
+    <row r="1158" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1158" s="1" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="B1158" s="1" t="s">
         <v>1611</v>
@@ -14968,66 +14965,66 @@
     </row>
     <row r="1159" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1159" s="1" t="s">
-        <v>33</v>
+        <v>34</v>
       </c>
       <c r="B1159" s="1" t="s">
         <v>1612</v>
       </c>
     </row>
-    <row r="1160" spans="1:10" ht="30" x14ac:dyDescent="0.25">
+    <row r="1160" spans="1:10" ht="270" x14ac:dyDescent="0.25">
       <c r="A1160" s="1" t="s">
-        <v>34</v>
+        <v>35</v>
       </c>
       <c r="B1160" s="1" t="s">
         <v>1613</v>
       </c>
-    </row>
-    <row r="1161" spans="1:10" ht="270" x14ac:dyDescent="0.25">
+      <c r="C1160" s="1" t="s">
+        <v>1757</v>
+      </c>
+      <c r="D1160" s="1" t="s">
+        <v>1758</v>
+      </c>
+      <c r="E1160" s="1" t="s">
+        <v>1759</v>
+      </c>
+      <c r="F1160" s="1" t="s">
+        <v>1760</v>
+      </c>
+      <c r="G1160" s="1" t="s">
+        <v>1761</v>
+      </c>
+      <c r="H1160" s="1" t="s">
+        <v>1762</v>
+      </c>
+      <c r="I1160" s="1" t="s">
+        <v>1763</v>
+      </c>
+      <c r="J1160" s="1" t="s">
+        <v>1764</v>
+      </c>
+    </row>
+    <row r="1161" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1161" s="1" t="s">
-        <v>35</v>
+        <v>36</v>
       </c>
       <c r="B1161" s="1" t="s">
-        <v>1614</v>
-      </c>
-      <c r="C1161" s="1" t="s">
-        <v>1758</v>
-      </c>
-      <c r="D1161" s="1" t="s">
-        <v>1759</v>
-      </c>
-      <c r="E1161" s="1" t="s">
-        <v>1760</v>
-      </c>
-      <c r="F1161" s="1" t="s">
-        <v>1761</v>
-      </c>
-      <c r="G1161" s="1" t="s">
-        <v>1762</v>
-      </c>
-      <c r="H1161" s="1" t="s">
-        <v>1763</v>
-      </c>
-      <c r="I1161" s="1" t="s">
-        <v>1764</v>
-      </c>
-      <c r="J1161" s="1" t="s">
-        <v>1765</v>
+        <v>36</v>
       </c>
     </row>
     <row r="1162" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1162" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B1162" s="1" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
     </row>
     <row r="1163" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A1163" s="1" t="s">
-        <v>37</v>
+        <v>1162</v>
       </c>
       <c r="B1163" s="1" t="s">
-        <v>37</v>
+        <v>1162</v>
       </c>
     </row>
     <row r="1164" spans="1:10" x14ac:dyDescent="0.25">
@@ -15038,31 +15035,31 @@
         <v>1163</v>
       </c>
     </row>
-    <row r="1165" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="1165" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1165" s="1" t="s">
-        <v>1164</v>
+        <v>1540</v>
       </c>
       <c r="B1165" s="1" t="s">
-        <v>1164</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="1166" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1166" s="1" t="s">
-        <v>1541</v>
+        <v>1614</v>
       </c>
       <c r="B1166" s="1" t="s">
-        <v>1689</v>
+        <v>1615</v>
       </c>
     </row>
     <row r="1167" spans="1:10" ht="45" x14ac:dyDescent="0.25">
       <c r="A1167" s="1" t="s">
+        <v>1164</v>
+      </c>
+      <c r="B1167" s="1" t="s">
         <v>1615</v>
       </c>
-      <c r="B1167" s="1" t="s">
-        <v>1616</v>
-      </c>
-    </row>
-    <row r="1168" spans="1:10" ht="45" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1168" spans="1:10" ht="30" x14ac:dyDescent="0.25">
       <c r="A1168" s="1" t="s">
         <v>1165</v>
       </c>
@@ -15078,7 +15075,7 @@
         <v>1617</v>
       </c>
     </row>
-    <row r="1170" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1170" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1170" s="1" t="s">
         <v>1167</v>
       </c>
@@ -15094,7 +15091,7 @@
         <v>1619</v>
       </c>
     </row>
-    <row r="1172" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1172" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1172" s="1" t="s">
         <v>1169</v>
       </c>
@@ -15102,7 +15099,7 @@
         <v>1620</v>
       </c>
     </row>
-    <row r="1173" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1173" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1173" s="1" t="s">
         <v>1170</v>
       </c>
@@ -15115,10 +15112,10 @@
         <v>1171</v>
       </c>
       <c r="B1174" s="1" t="s">
-        <v>1622</v>
-      </c>
-    </row>
-    <row r="1175" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1621</v>
+      </c>
+    </row>
+    <row r="1175" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1175" s="1" t="s">
         <v>1172</v>
       </c>
@@ -15131,7 +15128,7 @@
         <v>1173</v>
       </c>
       <c r="B1176" s="1" t="s">
-        <v>1623</v>
+        <v>1622</v>
       </c>
     </row>
     <row r="1177" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -15150,7 +15147,7 @@
         <v>1624</v>
       </c>
     </row>
-    <row r="1179" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1179" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1179" s="1" t="s">
         <v>1176</v>
       </c>
@@ -15158,7 +15155,7 @@
         <v>1625</v>
       </c>
     </row>
-    <row r="1180" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1180" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1180" s="1" t="s">
         <v>1177</v>
       </c>
@@ -15166,7 +15163,7 @@
         <v>1626</v>
       </c>
     </row>
-    <row r="1181" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1181" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1181" s="1" t="s">
         <v>1178</v>
       </c>
@@ -15174,7 +15171,7 @@
         <v>1627</v>
       </c>
     </row>
-    <row r="1182" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1182" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1182" s="1" t="s">
         <v>1179</v>
       </c>
@@ -15182,7 +15179,7 @@
         <v>1628</v>
       </c>
     </row>
-    <row r="1183" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1183" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1183" s="1" t="s">
         <v>1180</v>
       </c>
@@ -15198,7 +15195,7 @@
         <v>1630</v>
       </c>
     </row>
-    <row r="1185" spans="1:9" ht="45" x14ac:dyDescent="0.25">
+    <row r="1185" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1185" s="1" t="s">
         <v>1182</v>
       </c>
@@ -15219,10 +15216,10 @@
         <v>1184</v>
       </c>
       <c r="B1187" s="1" t="s">
-        <v>1633</v>
-      </c>
-    </row>
-    <row r="1188" spans="1:9" x14ac:dyDescent="0.25">
+        <v>1632</v>
+      </c>
+    </row>
+    <row r="1188" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1188" s="1" t="s">
         <v>1185</v>
       </c>
@@ -15243,10 +15240,10 @@
         <v>1187</v>
       </c>
       <c r="B1190" s="1" t="s">
-        <v>1635</v>
-      </c>
-    </row>
-    <row r="1191" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+        <v>1634</v>
+      </c>
+    </row>
+    <row r="1191" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A1191" s="1" t="s">
         <v>1188</v>
       </c>
@@ -15254,15 +15251,33 @@
         <v>1635</v>
       </c>
     </row>
-    <row r="1192" spans="1:9" ht="60" x14ac:dyDescent="0.25">
+    <row r="1192" spans="1:9" ht="315" x14ac:dyDescent="0.25">
       <c r="A1192" s="1" t="s">
         <v>1189</v>
       </c>
       <c r="B1192" s="1" t="s">
-        <v>1636</v>
-      </c>
-    </row>
-    <row r="1193" spans="1:9" ht="315" x14ac:dyDescent="0.25">
+        <v>1637</v>
+      </c>
+      <c r="C1192" s="1" t="s">
+        <v>1742</v>
+      </c>
+      <c r="D1192" s="1" t="s">
+        <v>1743</v>
+      </c>
+      <c r="E1192" s="1" t="s">
+        <v>1744</v>
+      </c>
+      <c r="F1192" s="1" t="s">
+        <v>1747</v>
+      </c>
+      <c r="G1192" s="1" t="s">
+        <v>1748</v>
+      </c>
+      <c r="H1192" s="1" t="s">
+        <v>1749</v>
+      </c>
+    </row>
+    <row r="1193" spans="1:9" ht="300" x14ac:dyDescent="0.25">
       <c r="A1193" s="1" t="s">
         <v>1190</v>
       </c>
@@ -15270,54 +15285,36 @@
         <v>1638</v>
       </c>
       <c r="C1193" s="1" t="s">
-        <v>1743</v>
+        <v>1750</v>
       </c>
       <c r="D1193" s="1" t="s">
-        <v>1744</v>
+        <v>1751</v>
       </c>
       <c r="E1193" s="1" t="s">
-        <v>1745</v>
+        <v>1752</v>
       </c>
       <c r="F1193" s="1" t="s">
-        <v>1748</v>
+        <v>1753</v>
       </c>
       <c r="G1193" s="1" t="s">
-        <v>1749</v>
+        <v>1754</v>
       </c>
       <c r="H1193" s="1" t="s">
-        <v>1750</v>
-      </c>
-    </row>
-    <row r="1194" spans="1:9" ht="300" x14ac:dyDescent="0.25">
+        <v>1755</v>
+      </c>
+      <c r="I1193" s="1" t="s">
+        <v>1756</v>
+      </c>
+    </row>
+    <row r="1194" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1194" s="1" t="s">
         <v>1191</v>
       </c>
       <c r="B1194" s="1" t="s">
         <v>1639</v>
       </c>
-      <c r="C1194" s="1" t="s">
-        <v>1751</v>
-      </c>
-      <c r="D1194" s="1" t="s">
-        <v>1752</v>
-      </c>
-      <c r="E1194" s="1" t="s">
-        <v>1753</v>
-      </c>
-      <c r="F1194" s="1" t="s">
-        <v>1754</v>
-      </c>
-      <c r="G1194" s="1" t="s">
-        <v>1755</v>
-      </c>
-      <c r="H1194" s="1" t="s">
-        <v>1756</v>
-      </c>
-      <c r="I1194" s="1" t="s">
-        <v>1757</v>
-      </c>
-    </row>
-    <row r="1195" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1195" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1195" s="1" t="s">
         <v>1192</v>
       </c>
@@ -15325,7 +15322,7 @@
         <v>1640</v>
       </c>
     </row>
-    <row r="1196" spans="1:9" x14ac:dyDescent="0.25">
+    <row r="1196" spans="1:9" ht="30" x14ac:dyDescent="0.25">
       <c r="A1196" s="1" t="s">
         <v>1193</v>
       </c>
@@ -15341,7 +15338,7 @@
         <v>1642</v>
       </c>
     </row>
-    <row r="1198" spans="1:9" ht="30" x14ac:dyDescent="0.25">
+    <row r="1198" spans="1:9" ht="105" x14ac:dyDescent="0.25">
       <c r="A1198" s="1" t="s">
         <v>1195</v>
       </c>
@@ -15349,7 +15346,7 @@
         <v>1643</v>
       </c>
     </row>
-    <row r="1199" spans="1:9" ht="105" x14ac:dyDescent="0.25">
+    <row r="1199" spans="1:9" ht="45" x14ac:dyDescent="0.25">
       <c r="A1199" s="1" t="s">
         <v>1196</v>
       </c>
@@ -15362,12 +15359,12 @@
         <v>1197</v>
       </c>
       <c r="B1200" s="1" t="s">
-        <v>1645</v>
-      </c>
-    </row>
-    <row r="1201" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>1644</v>
+      </c>
+    </row>
+    <row r="1201" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A1201" s="1" t="s">
-        <v>1198</v>
+        <v>1199</v>
       </c>
       <c r="B1201" s="1" t="s">
         <v>1645</v>
@@ -15375,15 +15372,15 @@
     </row>
     <row r="1202" spans="1:2" ht="90" x14ac:dyDescent="0.25">
       <c r="A1202" s="1" t="s">
+        <v>1198</v>
+      </c>
+      <c r="B1202" s="1" t="s">
+        <v>1645</v>
+      </c>
+    </row>
+    <row r="1203" spans="1:2" x14ac:dyDescent="0.25">
+      <c r="A1203" s="1" t="s">
         <v>1200</v>
-      </c>
-      <c r="B1202" s="1" t="s">
-        <v>1646</v>
-      </c>
-    </row>
-    <row r="1203" spans="1:2" ht="90" x14ac:dyDescent="0.25">
-      <c r="A1203" s="1" t="s">
-        <v>1199</v>
       </c>
       <c r="B1203" s="1" t="s">
         <v>1646</v>
@@ -15397,7 +15394,7 @@
         <v>1647</v>
       </c>
     </row>
-    <row r="1205" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1205" spans="1:2" ht="75" x14ac:dyDescent="0.25">
       <c r="A1205" s="1" t="s">
         <v>1202</v>
       </c>
@@ -15410,10 +15407,10 @@
         <v>1203</v>
       </c>
       <c r="B1206" s="1" t="s">
-        <v>1649</v>
-      </c>
-    </row>
-    <row r="1207" spans="1:2" ht="75" x14ac:dyDescent="0.25">
+        <v>1648</v>
+      </c>
+    </row>
+    <row r="1207" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1207" s="1" t="s">
         <v>1204</v>
       </c>
@@ -15421,7 +15418,7 @@
         <v>1649</v>
       </c>
     </row>
-    <row r="1208" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1208" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1208" s="1" t="s">
         <v>1205</v>
       </c>
@@ -15431,7 +15428,7 @@
     </row>
     <row r="1209" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1209" s="1" t="s">
-        <v>1206</v>
+        <v>1299</v>
       </c>
       <c r="B1209" s="1" t="s">
         <v>1651</v>
@@ -15439,29 +15436,29 @@
     </row>
     <row r="1210" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1210" s="1" t="s">
-        <v>1300</v>
+        <v>1208</v>
       </c>
       <c r="B1210" s="1" t="s">
         <v>1652</v>
       </c>
     </row>
-    <row r="1211" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1211" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1211" s="1" t="s">
-        <v>1209</v>
+        <v>1207</v>
       </c>
       <c r="B1211" s="1" t="s">
         <v>1653</v>
       </c>
     </row>
-    <row r="1212" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1212" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1212" s="1" t="s">
-        <v>1208</v>
+        <v>1300</v>
       </c>
       <c r="B1212" s="1" t="s">
         <v>1654</v>
       </c>
     </row>
-    <row r="1213" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1213" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1213" s="1" t="s">
         <v>1301</v>
       </c>
@@ -15469,7 +15466,7 @@
         <v>1655</v>
       </c>
     </row>
-    <row r="1214" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1214" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1214" s="1" t="s">
         <v>1302</v>
       </c>
@@ -15509,44 +15506,44 @@
         <v>1660</v>
       </c>
     </row>
-    <row r="1219" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1219" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1219" s="1" t="s">
+        <v>1206</v>
+      </c>
+      <c r="B1219" s="1" t="s">
+        <v>1605</v>
+      </c>
+    </row>
+    <row r="1220" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1220" s="1" t="s">
         <v>1307</v>
       </c>
-      <c r="B1219" s="1" t="s">
-        <v>1661</v>
-      </c>
-    </row>
-    <row r="1220" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1220" s="1" t="s">
-        <v>1207</v>
-      </c>
       <c r="B1220" s="1" t="s">
-        <v>1606</v>
+        <v>1599</v>
       </c>
     </row>
     <row r="1221" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1221" s="1" t="s">
-        <v>1308</v>
+        <v>1209</v>
       </c>
       <c r="B1221" s="1" t="s">
-        <v>1600</v>
-      </c>
-    </row>
-    <row r="1222" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1534</v>
+      </c>
+    </row>
+    <row r="1222" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1222" s="1" t="s">
         <v>1210</v>
       </c>
-      <c r="B1222" s="1" t="s">
-        <v>1535</v>
+      <c r="B1222" t="s">
+        <v>1533</v>
       </c>
     </row>
     <row r="1223" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1223" s="1" t="s">
         <v>1211</v>
       </c>
-      <c r="B1223" t="s">
-        <v>1534</v>
+      <c r="B1223" s="1" t="s">
+        <v>1703</v>
       </c>
     </row>
     <row r="1224" spans="1:2" x14ac:dyDescent="0.25">
@@ -15578,7 +15575,7 @@
         <v>1215</v>
       </c>
       <c r="B1227" s="1" t="s">
-        <v>1707</v>
+        <v>1705</v>
       </c>
     </row>
     <row r="1228" spans="1:2" x14ac:dyDescent="0.25">
@@ -15586,7 +15583,7 @@
         <v>1216</v>
       </c>
       <c r="B1228" s="1" t="s">
-        <v>1706</v>
+        <v>1704</v>
       </c>
     </row>
     <row r="1229" spans="1:2" x14ac:dyDescent="0.25">
@@ -15594,7 +15591,7 @@
         <v>1217</v>
       </c>
       <c r="B1229" s="1" t="s">
-        <v>1705</v>
+        <v>1698</v>
       </c>
     </row>
     <row r="1230" spans="1:2" x14ac:dyDescent="0.25">
@@ -15602,7 +15599,7 @@
         <v>1218</v>
       </c>
       <c r="B1230" s="1" t="s">
-        <v>1699</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1231" spans="1:2" x14ac:dyDescent="0.25">
@@ -15610,7 +15607,7 @@
         <v>1219</v>
       </c>
       <c r="B1231" s="1" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1232" spans="1:2" x14ac:dyDescent="0.25">
@@ -15618,7 +15615,7 @@
         <v>1220</v>
       </c>
       <c r="B1232" s="1" t="s">
-        <v>1548</v>
+        <v>1547</v>
       </c>
     </row>
     <row r="1233" spans="1:2" x14ac:dyDescent="0.25">
@@ -15634,7 +15631,7 @@
         <v>1222</v>
       </c>
       <c r="B1234" s="1" t="s">
-        <v>1549</v>
+        <v>1548</v>
       </c>
     </row>
     <row r="1235" spans="1:2" x14ac:dyDescent="0.25">
@@ -15642,7 +15639,7 @@
         <v>1223</v>
       </c>
       <c r="B1235" s="1" t="s">
-        <v>1549</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="1236" spans="1:2" x14ac:dyDescent="0.25">
@@ -15650,7 +15647,7 @@
         <v>1224</v>
       </c>
       <c r="B1236" s="1" t="s">
-        <v>1690</v>
+        <v>1689</v>
       </c>
     </row>
     <row r="1237" spans="1:2" x14ac:dyDescent="0.25">
@@ -15658,10 +15655,10 @@
         <v>1225</v>
       </c>
       <c r="B1237" s="1" t="s">
-        <v>1690</v>
-      </c>
-    </row>
-    <row r="1238" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1681</v>
+      </c>
+    </row>
+    <row r="1238" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1238" s="1" t="s">
         <v>1226</v>
       </c>
@@ -15677,7 +15674,7 @@
         <v>1683</v>
       </c>
     </row>
-    <row r="1240" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1240" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1240" s="1" t="s">
         <v>1228</v>
       </c>
@@ -15685,12 +15682,12 @@
         <v>1684</v>
       </c>
     </row>
-    <row r="1241" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1241" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1241" s="1" t="s">
         <v>1229</v>
       </c>
       <c r="B1241" s="1" t="s">
-        <v>1685</v>
+        <v>1682</v>
       </c>
     </row>
     <row r="1242" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -15701,12 +15698,12 @@
         <v>1683</v>
       </c>
     </row>
-    <row r="1243" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1243" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1243" s="1" t="s">
         <v>1231</v>
       </c>
       <c r="B1243" s="1" t="s">
-        <v>1684</v>
+        <v>1675</v>
       </c>
     </row>
     <row r="1244" spans="1:2" x14ac:dyDescent="0.25">
@@ -15714,15 +15711,15 @@
         <v>1232</v>
       </c>
       <c r="B1244" s="1" t="s">
-        <v>1676</v>
-      </c>
-    </row>
-    <row r="1245" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1675</v>
+      </c>
+    </row>
+    <row r="1245" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1245" s="1" t="s">
         <v>1233</v>
       </c>
       <c r="B1245" s="1" t="s">
-        <v>1676</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="1246" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -15730,7 +15727,7 @@
         <v>1234</v>
       </c>
       <c r="B1246" s="1" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="1247" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -15738,7 +15735,7 @@
         <v>1235</v>
       </c>
       <c r="B1247" s="1" t="s">
-        <v>1713</v>
+        <v>1712</v>
       </c>
     </row>
     <row r="1248" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -15746,23 +15743,23 @@
         <v>1236</v>
       </c>
       <c r="B1248" s="1" t="s">
-        <v>1713</v>
-      </c>
-    </row>
-    <row r="1249" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1712</v>
+      </c>
+    </row>
+    <row r="1249" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1249" s="1" t="s">
         <v>1237</v>
       </c>
       <c r="B1249" s="1" t="s">
-        <v>1713</v>
-      </c>
-    </row>
-    <row r="1250" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1711</v>
+      </c>
+    </row>
+    <row r="1250" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1250" s="1" t="s">
         <v>1238</v>
       </c>
       <c r="B1250" s="1" t="s">
-        <v>1712</v>
+        <v>1713</v>
       </c>
     </row>
     <row r="1251" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -15778,15 +15775,15 @@
         <v>1240</v>
       </c>
       <c r="B1252" s="1" t="s">
-        <v>1715</v>
-      </c>
-    </row>
-    <row r="1253" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>1713</v>
+      </c>
+    </row>
+    <row r="1253" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1253" s="1" t="s">
         <v>1241</v>
       </c>
       <c r="B1253" s="1" t="s">
-        <v>1714</v>
+        <v>1551</v>
       </c>
     </row>
     <row r="1254" spans="1:2" x14ac:dyDescent="0.25">
@@ -15794,7 +15791,7 @@
         <v>1242</v>
       </c>
       <c r="B1254" s="1" t="s">
-        <v>1552</v>
+        <v>1715</v>
       </c>
     </row>
     <row r="1255" spans="1:2" x14ac:dyDescent="0.25">
@@ -15802,23 +15799,23 @@
         <v>1243</v>
       </c>
       <c r="B1255" s="1" t="s">
-        <v>1716</v>
-      </c>
-    </row>
-    <row r="1256" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1551</v>
+      </c>
+    </row>
+    <row r="1256" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1256" s="1" t="s">
         <v>1244</v>
       </c>
       <c r="B1256" s="1" t="s">
-        <v>1552</v>
-      </c>
-    </row>
-    <row r="1257" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="1257" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1257" s="1" t="s">
         <v>1245</v>
       </c>
       <c r="B1257" s="1" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="1258" spans="1:2" x14ac:dyDescent="0.25">
@@ -15826,23 +15823,23 @@
         <v>1246</v>
       </c>
       <c r="B1258" s="1" t="s">
-        <v>1718</v>
-      </c>
-    </row>
-    <row r="1259" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1716</v>
+      </c>
+    </row>
+    <row r="1259" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1259" s="1" t="s">
         <v>1247</v>
       </c>
       <c r="B1259" s="1" t="s">
-        <v>1717</v>
-      </c>
-    </row>
-    <row r="1260" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>1718</v>
+      </c>
+    </row>
+    <row r="1260" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1260" s="1" t="s">
         <v>1248</v>
       </c>
       <c r="B1260" s="1" t="s">
-        <v>1719</v>
+        <v>1717</v>
       </c>
     </row>
     <row r="1261" spans="1:2" x14ac:dyDescent="0.25">
@@ -15850,7 +15847,7 @@
         <v>1249</v>
       </c>
       <c r="B1261" s="1" t="s">
-        <v>1718</v>
+        <v>1716</v>
       </c>
     </row>
     <row r="1262" spans="1:2" x14ac:dyDescent="0.25">
@@ -15858,10 +15855,10 @@
         <v>1250</v>
       </c>
       <c r="B1262" s="1" t="s">
-        <v>1717</v>
-      </c>
-    </row>
-    <row r="1263" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="1263" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1263" s="1" t="s">
         <v>1251</v>
       </c>
@@ -15874,18 +15871,18 @@
         <v>1252</v>
       </c>
       <c r="B1264" s="1" t="s">
-        <v>1721</v>
-      </c>
-    </row>
-    <row r="1265" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1720</v>
+      </c>
+    </row>
+    <row r="1265" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1265" s="1" t="s">
         <v>1253</v>
       </c>
       <c r="B1265" s="1" t="s">
-        <v>1721</v>
-      </c>
-    </row>
-    <row r="1266" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1719</v>
+      </c>
+    </row>
+    <row r="1266" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1266" s="1" t="s">
         <v>1254</v>
       </c>
@@ -15893,12 +15890,12 @@
         <v>1720</v>
       </c>
     </row>
-    <row r="1267" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1267" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1267" s="1" t="s">
         <v>1255</v>
       </c>
       <c r="B1267" s="1" t="s">
-        <v>1721</v>
+        <v>1719</v>
       </c>
     </row>
     <row r="1268" spans="1:2" x14ac:dyDescent="0.25">
@@ -15906,7 +15903,7 @@
         <v>1256</v>
       </c>
       <c r="B1268" s="1" t="s">
-        <v>1720</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="1269" spans="1:2" x14ac:dyDescent="0.25">
@@ -15922,7 +15919,7 @@
         <v>1258</v>
       </c>
       <c r="B1270" s="1" t="s">
-        <v>1724</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="1271" spans="1:2" x14ac:dyDescent="0.25">
@@ -15930,7 +15927,7 @@
         <v>1259</v>
       </c>
       <c r="B1271" s="1" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="1272" spans="1:2" x14ac:dyDescent="0.25">
@@ -15938,7 +15935,7 @@
         <v>1260</v>
       </c>
       <c r="B1272" s="1" t="s">
-        <v>1723</v>
+        <v>1722</v>
       </c>
     </row>
     <row r="1273" spans="1:2" x14ac:dyDescent="0.25">
@@ -15946,7 +15943,7 @@
         <v>1261</v>
       </c>
       <c r="B1273" s="1" t="s">
-        <v>1723</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="1274" spans="1:2" x14ac:dyDescent="0.25">
@@ -15957,20 +15954,20 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="1275" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1275" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1275" s="1" t="s">
         <v>1263</v>
       </c>
       <c r="B1275" s="1" t="s">
-        <v>1726</v>
-      </c>
-    </row>
-    <row r="1276" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1683</v>
+      </c>
+    </row>
+    <row r="1276" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1276" s="1" t="s">
         <v>1264</v>
       </c>
       <c r="B1276" s="1" t="s">
-        <v>1684</v>
+        <v>1724</v>
       </c>
     </row>
     <row r="1277" spans="1:2" x14ac:dyDescent="0.25">
@@ -15981,12 +15978,12 @@
         <v>1725</v>
       </c>
     </row>
-    <row r="1278" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1278" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1278" s="1" t="s">
         <v>1266</v>
       </c>
       <c r="B1278" s="1" t="s">
-        <v>1726</v>
+        <v>1683</v>
       </c>
     </row>
     <row r="1279" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -15994,15 +15991,15 @@
         <v>1267</v>
       </c>
       <c r="B1279" s="1" t="s">
-        <v>1684</v>
-      </c>
-    </row>
-    <row r="1280" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="1280" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1280" s="1" t="s">
         <v>1268</v>
       </c>
       <c r="B1280" s="1" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="1281" spans="1:2" x14ac:dyDescent="0.25">
@@ -16010,23 +16007,23 @@
         <v>1269</v>
       </c>
       <c r="B1281" s="1" t="s">
-        <v>1727</v>
-      </c>
-    </row>
-    <row r="1282" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="1282" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1282" s="1" t="s">
         <v>1270</v>
       </c>
       <c r="B1282" s="1" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="1283" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1727</v>
+      </c>
+    </row>
+    <row r="1283" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1283" s="1" t="s">
         <v>1271</v>
       </c>
       <c r="B1283" s="1" t="s">
-        <v>1728</v>
+        <v>1726</v>
       </c>
     </row>
     <row r="1284" spans="1:2" x14ac:dyDescent="0.25">
@@ -16034,31 +16031,31 @@
         <v>1272</v>
       </c>
       <c r="B1284" s="1" t="s">
-        <v>1727</v>
-      </c>
-    </row>
-    <row r="1285" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1552</v>
+      </c>
+    </row>
+    <row r="1285" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1285" s="1" t="s">
         <v>1273</v>
       </c>
       <c r="B1285" s="1" t="s">
-        <v>1553</v>
-      </c>
-    </row>
-    <row r="1286" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="1286" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1286" s="1" t="s">
         <v>1274</v>
       </c>
       <c r="B1286" s="1" t="s">
-        <v>1729</v>
-      </c>
-    </row>
-    <row r="1287" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="1287" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1287" s="1" t="s">
         <v>1275</v>
       </c>
       <c r="B1287" s="1" t="s">
-        <v>1731</v>
+        <v>1729</v>
       </c>
     </row>
     <row r="1288" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16066,31 +16063,31 @@
         <v>1276</v>
       </c>
       <c r="B1288" s="1" t="s">
-        <v>1730</v>
-      </c>
-    </row>
-    <row r="1289" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1728</v>
+      </c>
+    </row>
+    <row r="1289" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1289" s="1" t="s">
         <v>1277</v>
       </c>
       <c r="B1289" s="1" t="s">
-        <v>1729</v>
-      </c>
-    </row>
-    <row r="1290" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1730</v>
+      </c>
+    </row>
+    <row r="1290" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1290" s="1" t="s">
         <v>1278</v>
       </c>
       <c r="B1290" s="1" t="s">
-        <v>1731</v>
-      </c>
-    </row>
-    <row r="1291" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1729</v>
+      </c>
+    </row>
+    <row r="1291" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1291" s="1" t="s">
         <v>1279</v>
       </c>
       <c r="B1291" s="1" t="s">
-        <v>1730</v>
+        <v>1707</v>
       </c>
     </row>
     <row r="1292" spans="1:2" x14ac:dyDescent="0.25">
@@ -16101,12 +16098,12 @@
         <v>1708</v>
       </c>
     </row>
-    <row r="1293" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1293" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1293" s="1" t="s">
         <v>1281</v>
       </c>
       <c r="B1293" s="1" t="s">
-        <v>1709</v>
+        <v>1701</v>
       </c>
     </row>
     <row r="1294" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16114,15 +16111,15 @@
         <v>1282</v>
       </c>
       <c r="B1294" s="1" t="s">
-        <v>1702</v>
-      </c>
-    </row>
-    <row r="1295" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1701</v>
+      </c>
+    </row>
+    <row r="1295" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1295" s="1" t="s">
         <v>1283</v>
       </c>
       <c r="B1295" s="1" t="s">
-        <v>1702</v>
+        <v>1699</v>
       </c>
     </row>
     <row r="1296" spans="1:2" x14ac:dyDescent="0.25">
@@ -16130,7 +16127,7 @@
         <v>1284</v>
       </c>
       <c r="B1296" s="1" t="s">
-        <v>1700</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="1297" spans="1:2" x14ac:dyDescent="0.25">
@@ -16138,7 +16135,7 @@
         <v>1285</v>
       </c>
       <c r="B1297" s="1" t="s">
-        <v>1703</v>
+        <v>1702</v>
       </c>
     </row>
     <row r="1298" spans="1:2" x14ac:dyDescent="0.25">
@@ -16146,7 +16143,7 @@
         <v>1286</v>
       </c>
       <c r="B1298" s="1" t="s">
-        <v>1703</v>
+        <v>1697</v>
       </c>
     </row>
     <row r="1299" spans="1:2" x14ac:dyDescent="0.25">
@@ -16154,7 +16151,7 @@
         <v>1287</v>
       </c>
       <c r="B1299" s="1" t="s">
-        <v>1698</v>
+        <v>1693</v>
       </c>
     </row>
     <row r="1300" spans="1:2" x14ac:dyDescent="0.25">
@@ -16162,10 +16159,10 @@
         <v>1288</v>
       </c>
       <c r="B1300" s="1" t="s">
-        <v>1694</v>
-      </c>
-    </row>
-    <row r="1301" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1693</v>
+      </c>
+    </row>
+    <row r="1301" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1301" s="1" t="s">
         <v>1289</v>
       </c>
@@ -16194,7 +16191,7 @@
         <v>1292</v>
       </c>
       <c r="B1304" s="1" t="s">
-        <v>1697</v>
+        <v>1696</v>
       </c>
     </row>
     <row r="1305" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16202,15 +16199,15 @@
         <v>1293</v>
       </c>
       <c r="B1305" s="1" t="s">
-        <v>1697</v>
-      </c>
-    </row>
-    <row r="1306" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1685</v>
+      </c>
+    </row>
+    <row r="1306" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1306" s="1" t="s">
         <v>1294</v>
       </c>
       <c r="B1306" s="1" t="s">
-        <v>1686</v>
+        <v>1688</v>
       </c>
     </row>
     <row r="1307" spans="1:2" ht="45" x14ac:dyDescent="0.25">
@@ -16218,15 +16215,15 @@
         <v>1295</v>
       </c>
       <c r="B1307" s="1" t="s">
-        <v>1689</v>
-      </c>
-    </row>
-    <row r="1308" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>1688</v>
+      </c>
+    </row>
+    <row r="1308" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1308" s="1" t="s">
         <v>1296</v>
       </c>
       <c r="B1308" s="1" t="s">
-        <v>1689</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="1309" spans="1:2" x14ac:dyDescent="0.25">
@@ -16234,7 +16231,7 @@
         <v>1297</v>
       </c>
       <c r="B1309" s="1" t="s">
-        <v>1688</v>
+        <v>1687</v>
       </c>
     </row>
     <row r="1310" spans="1:2" x14ac:dyDescent="0.25">
@@ -16242,15 +16239,15 @@
         <v>1298</v>
       </c>
       <c r="B1310" s="1" t="s">
-        <v>1688</v>
+        <v>1298</v>
       </c>
     </row>
     <row r="1311" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1311" s="1" t="s">
-        <v>1299</v>
+        <v>1308</v>
       </c>
       <c r="B1311" s="1" t="s">
-        <v>1299</v>
+        <v>1563</v>
       </c>
     </row>
     <row r="1312" spans="1:2" x14ac:dyDescent="0.25">
@@ -16258,7 +16255,7 @@
         <v>1309</v>
       </c>
       <c r="B1312" s="1" t="s">
-        <v>1564</v>
+        <v>1309</v>
       </c>
     </row>
     <row r="1313" spans="1:2" x14ac:dyDescent="0.25">
@@ -16770,7 +16767,7 @@
         <v>1373</v>
       </c>
       <c r="B1376" s="1" t="s">
-        <v>1373</v>
+        <v>1514</v>
       </c>
     </row>
     <row r="1377" spans="1:2" x14ac:dyDescent="0.25">
@@ -16778,7 +16775,7 @@
         <v>1374</v>
       </c>
       <c r="B1377" s="1" t="s">
-        <v>1515</v>
+        <v>1374</v>
       </c>
     </row>
     <row r="1378" spans="1:2" x14ac:dyDescent="0.25">
@@ -16813,20 +16810,20 @@
         <v>1378</v>
       </c>
     </row>
-    <row r="1382" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1382" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1382" s="1" t="s">
         <v>1379</v>
       </c>
       <c r="B1382" s="1" t="s">
-        <v>1379</v>
-      </c>
-    </row>
-    <row r="1383" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1652</v>
+      </c>
+    </row>
+    <row r="1383" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1383" s="1" t="s">
         <v>1380</v>
       </c>
       <c r="B1383" s="1" t="s">
-        <v>1653</v>
+        <v>1380</v>
       </c>
     </row>
     <row r="1384" spans="1:2" x14ac:dyDescent="0.25">
@@ -16837,12 +16834,12 @@
         <v>1381</v>
       </c>
     </row>
-    <row r="1385" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1385" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1385" s="1" t="s">
         <v>1382</v>
       </c>
       <c r="B1385" s="1" t="s">
-        <v>1382</v>
+        <v>1661</v>
       </c>
     </row>
     <row r="1386" spans="1:2" ht="30" x14ac:dyDescent="0.25">
@@ -16861,12 +16858,12 @@
         <v>1663</v>
       </c>
     </row>
-    <row r="1388" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1388" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1388" s="1" t="s">
         <v>1385</v>
       </c>
       <c r="B1388" s="1" t="s">
-        <v>1664</v>
+        <v>1385</v>
       </c>
     </row>
     <row r="1389" spans="1:2" x14ac:dyDescent="0.25">
@@ -16877,20 +16874,20 @@
         <v>1386</v>
       </c>
     </row>
-    <row r="1390" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1390" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1390" s="1" t="s">
         <v>1387</v>
       </c>
       <c r="B1390" s="1" t="s">
-        <v>1387</v>
-      </c>
-    </row>
-    <row r="1391" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>1669</v>
+      </c>
+    </row>
+    <row r="1391" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1391" s="1" t="s">
         <v>1388</v>
       </c>
       <c r="B1391" s="1" t="s">
-        <v>1670</v>
+        <v>1388</v>
       </c>
     </row>
     <row r="1392" spans="1:2" x14ac:dyDescent="0.25">
@@ -16906,7 +16903,7 @@
         <v>1390</v>
       </c>
       <c r="B1393" s="1" t="s">
-        <v>1390</v>
+        <v>1632</v>
       </c>
     </row>
     <row r="1394" spans="1:2" x14ac:dyDescent="0.25">
@@ -16914,18 +16911,18 @@
         <v>1391</v>
       </c>
       <c r="B1394" s="1" t="s">
-        <v>1633</v>
-      </c>
-    </row>
-    <row r="1395" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1391</v>
+      </c>
+    </row>
+    <row r="1395" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1395" s="1" t="s">
         <v>1392</v>
       </c>
       <c r="B1395" s="1" t="s">
-        <v>1392</v>
-      </c>
-    </row>
-    <row r="1396" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1664</v>
+      </c>
+    </row>
+    <row r="1396" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1396" s="1" t="s">
         <v>1393</v>
       </c>
@@ -16933,12 +16930,12 @@
         <v>1665</v>
       </c>
     </row>
-    <row r="1397" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+    <row r="1397" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1397" s="1" t="s">
         <v>1394</v>
       </c>
       <c r="B1397" s="1" t="s">
-        <v>1666</v>
+        <v>1394</v>
       </c>
     </row>
     <row r="1398" spans="1:2" x14ac:dyDescent="0.25">
@@ -16957,20 +16954,20 @@
         <v>1396</v>
       </c>
     </row>
-    <row r="1400" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1400" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1400" s="1" t="s">
         <v>1397</v>
       </c>
       <c r="B1400" s="1" t="s">
-        <v>1397</v>
-      </c>
-    </row>
-    <row r="1401" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1666</v>
+      </c>
+    </row>
+    <row r="1401" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1401" s="1" t="s">
         <v>1398</v>
       </c>
       <c r="B1401" s="1" t="s">
-        <v>1667</v>
+        <v>1398</v>
       </c>
     </row>
     <row r="1402" spans="1:2" x14ac:dyDescent="0.25">
@@ -16997,20 +16994,20 @@
         <v>1401</v>
       </c>
     </row>
-    <row r="1405" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1405" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1405" s="1" t="s">
         <v>1402</v>
       </c>
       <c r="B1405" s="1" t="s">
-        <v>1402</v>
-      </c>
-    </row>
-    <row r="1406" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1667</v>
+      </c>
+    </row>
+    <row r="1406" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1406" s="1" t="s">
         <v>1403</v>
       </c>
       <c r="B1406" s="1" t="s">
-        <v>1668</v>
+        <v>1403</v>
       </c>
     </row>
     <row r="1407" spans="1:2" x14ac:dyDescent="0.25">
@@ -17037,20 +17034,20 @@
         <v>1406</v>
       </c>
     </row>
-    <row r="1410" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1410" spans="1:2" ht="45" x14ac:dyDescent="0.25">
       <c r="A1410" s="1" t="s">
         <v>1407</v>
       </c>
       <c r="B1410" s="1" t="s">
-        <v>1407</v>
-      </c>
-    </row>
-    <row r="1411" spans="1:2" ht="45" x14ac:dyDescent="0.25">
+        <v>1668</v>
+      </c>
+    </row>
+    <row r="1411" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1411" s="1" t="s">
         <v>1408</v>
       </c>
       <c r="B1411" s="1" t="s">
-        <v>1669</v>
+        <v>1408</v>
       </c>
     </row>
     <row r="1412" spans="1:2" x14ac:dyDescent="0.25">
@@ -17122,7 +17119,7 @@
         <v>1417</v>
       </c>
       <c r="B1420" s="1" t="s">
-        <v>1417</v>
+        <v>1524</v>
       </c>
     </row>
     <row r="1421" spans="1:2" x14ac:dyDescent="0.25">
@@ -17130,23 +17127,23 @@
         <v>1418</v>
       </c>
       <c r="B1421" s="1" t="s">
-        <v>1525</v>
-      </c>
-    </row>
-    <row r="1422" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1418</v>
+      </c>
+    </row>
+    <row r="1422" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1422" s="1" t="s">
         <v>1419</v>
       </c>
       <c r="B1422" s="1" t="s">
-        <v>1419</v>
-      </c>
-    </row>
-    <row r="1423" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1525</v>
+      </c>
+    </row>
+    <row r="1423" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1423" s="1" t="s">
         <v>1420</v>
       </c>
       <c r="B1423" s="1" t="s">
-        <v>1526</v>
+        <v>1420</v>
       </c>
     </row>
     <row r="1424" spans="1:2" x14ac:dyDescent="0.25">
@@ -17197,7 +17194,7 @@
         <v>1426</v>
       </c>
     </row>
-    <row r="1430" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1430" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1430" s="1" t="s">
         <v>1427</v>
       </c>
@@ -17205,7 +17202,7 @@
         <v>1427</v>
       </c>
     </row>
-    <row r="1431" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1431" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1431" s="1" t="s">
         <v>1428</v>
       </c>
@@ -17229,7 +17226,7 @@
         <v>1430</v>
       </c>
     </row>
-    <row r="1434" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1434" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1434" s="1" t="s">
         <v>1431</v>
       </c>
@@ -17237,7 +17234,7 @@
         <v>1431</v>
       </c>
     </row>
-    <row r="1435" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1435" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1435" s="1" t="s">
         <v>1432</v>
       </c>
@@ -17250,7 +17247,7 @@
         <v>1433</v>
       </c>
       <c r="B1436" s="1" t="s">
-        <v>1433</v>
+        <v>1636</v>
       </c>
     </row>
     <row r="1437" spans="1:2" x14ac:dyDescent="0.25">
@@ -17258,7 +17255,7 @@
         <v>1434</v>
       </c>
       <c r="B1437" s="1" t="s">
-        <v>1637</v>
+        <v>1434</v>
       </c>
     </row>
     <row r="1438" spans="1:2" x14ac:dyDescent="0.25">
@@ -17482,7 +17479,7 @@
         <v>1462</v>
       </c>
       <c r="B1465" s="1" t="s">
-        <v>1462</v>
+        <v>1532</v>
       </c>
     </row>
     <row r="1466" spans="1:2" x14ac:dyDescent="0.25">
@@ -17490,7 +17487,7 @@
         <v>1463</v>
       </c>
       <c r="B1466" s="1" t="s">
-        <v>1533</v>
+        <v>1463</v>
       </c>
     </row>
     <row r="1467" spans="1:2" x14ac:dyDescent="0.25">
@@ -17557,7 +17554,7 @@
         <v>1471</v>
       </c>
     </row>
-    <row r="1475" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1475" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1475" s="1" t="s">
         <v>1472</v>
       </c>
@@ -17565,7 +17562,7 @@
         <v>1472</v>
       </c>
     </row>
-    <row r="1476" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1476" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1476" s="1" t="s">
         <v>1473</v>
       </c>
@@ -17658,23 +17655,23 @@
         <v>1484</v>
       </c>
       <c r="B1487" s="1" t="s">
-        <v>1484</v>
-      </c>
-    </row>
-    <row r="1488" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1511</v>
+      </c>
+    </row>
+    <row r="1488" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1488" s="1" t="s">
         <v>1485</v>
       </c>
       <c r="B1488" s="1" t="s">
-        <v>1512</v>
-      </c>
-    </row>
-    <row r="1489" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1510</v>
+      </c>
+    </row>
+    <row r="1489" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1489" s="1" t="s">
         <v>1486</v>
       </c>
       <c r="B1489" s="1" t="s">
-        <v>1511</v>
+        <v>1486</v>
       </c>
     </row>
     <row r="1490" spans="1:2" x14ac:dyDescent="0.25">
@@ -17687,18 +17684,18 @@
     </row>
     <row r="1491" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1491" s="1" t="s">
-        <v>1488</v>
+        <v>1528</v>
       </c>
       <c r="B1491" s="1" t="s">
-        <v>1488</v>
+        <v>1529</v>
       </c>
     </row>
     <row r="1492" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1492" s="1" t="s">
-        <v>1529</v>
+        <v>1501</v>
       </c>
       <c r="B1492" s="1" t="s">
-        <v>1530</v>
+        <v>1501</v>
       </c>
     </row>
     <row r="1493" spans="1:2" x14ac:dyDescent="0.25">
@@ -17706,12 +17703,12 @@
         <v>1502</v>
       </c>
       <c r="B1493" s="1" t="s">
-        <v>1502</v>
+        <v>1503</v>
       </c>
     </row>
     <row r="1494" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1494" s="1" t="s">
-        <v>1503</v>
+        <v>1504</v>
       </c>
       <c r="B1494" s="1" t="s">
         <v>1504</v>
@@ -17722,12 +17719,12 @@
         <v>1505</v>
       </c>
       <c r="B1495" s="1" t="s">
-        <v>1505</v>
+        <v>1506</v>
       </c>
     </row>
     <row r="1496" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1496" s="1" t="s">
-        <v>1506</v>
+        <v>1507</v>
       </c>
       <c r="B1496" s="1" t="s">
         <v>1507</v>
@@ -17738,20 +17735,20 @@
         <v>1508</v>
       </c>
       <c r="B1497" s="1" t="s">
-        <v>1508</v>
+        <v>1509</v>
       </c>
     </row>
     <row r="1498" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1498" s="1" t="s">
-        <v>1509</v>
+        <v>1512</v>
       </c>
       <c r="B1498" s="1" t="s">
-        <v>1510</v>
+        <v>1512</v>
       </c>
     </row>
     <row r="1499" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1499" s="1" t="s">
-        <v>1513</v>
+        <v>1518</v>
       </c>
       <c r="B1499" s="1" t="s">
         <v>1513</v>
@@ -17759,7 +17756,7 @@
     </row>
     <row r="1500" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1500" s="1" t="s">
-        <v>1519</v>
+        <v>1515</v>
       </c>
       <c r="B1500" s="1" t="s">
         <v>1514</v>
@@ -17770,7 +17767,7 @@
         <v>1516</v>
       </c>
       <c r="B1501" s="1" t="s">
-        <v>1515</v>
+        <v>1516</v>
       </c>
     </row>
     <row r="1502" spans="1:2" x14ac:dyDescent="0.25">
@@ -17778,74 +17775,74 @@
         <v>1517</v>
       </c>
       <c r="B1502" s="1" t="s">
-        <v>1517</v>
+        <v>1519</v>
       </c>
     </row>
     <row r="1503" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1503" s="1" t="s">
-        <v>1518</v>
+        <v>1520</v>
       </c>
       <c r="B1503" s="1" t="s">
-        <v>1520</v>
+        <v>1521</v>
       </c>
     </row>
     <row r="1504" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1504" s="1" t="s">
-        <v>1521</v>
+        <v>1377</v>
       </c>
       <c r="B1504" s="1" t="s">
-        <v>1522</v>
+        <v>1377</v>
       </c>
     </row>
     <row r="1505" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1505" s="1" t="s">
-        <v>1378</v>
+        <v>1487</v>
       </c>
       <c r="B1505" s="1" t="s">
-        <v>1378</v>
+        <v>1522</v>
       </c>
     </row>
     <row r="1506" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1506" s="1" t="s">
-        <v>1488</v>
+        <v>1376</v>
       </c>
       <c r="B1506" s="1" t="s">
-        <v>1523</v>
+        <v>1376</v>
       </c>
     </row>
     <row r="1507" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1507" s="1" t="s">
-        <v>1377</v>
+        <v>1486</v>
       </c>
       <c r="B1507" s="1" t="s">
-        <v>1377</v>
+        <v>1523</v>
       </c>
     </row>
     <row r="1508" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1508" s="1" t="s">
-        <v>1487</v>
+        <v>1526</v>
       </c>
       <c r="B1508" s="1" t="s">
-        <v>1524</v>
+        <v>1527</v>
       </c>
     </row>
     <row r="1509" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1509" s="1" t="s">
-        <v>1527</v>
+        <v>1530</v>
       </c>
       <c r="B1509" s="1" t="s">
-        <v>1528</v>
-      </c>
-    </row>
-    <row r="1510" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1531</v>
+      </c>
+    </row>
+    <row r="1510" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1510" s="1" t="s">
-        <v>1531</v>
+        <v>1535</v>
       </c>
       <c r="B1510" s="1" t="s">
-        <v>1532</v>
-      </c>
-    </row>
-    <row r="1511" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1676</v>
+      </c>
+    </row>
+    <row r="1511" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1511" s="1" t="s">
         <v>1536</v>
       </c>
@@ -17861,7 +17858,7 @@
         <v>1678</v>
       </c>
     </row>
-    <row r="1513" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1513" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1513" s="1" t="s">
         <v>1538</v>
       </c>
@@ -17877,12 +17874,12 @@
         <v>1680</v>
       </c>
     </row>
-    <row r="1515" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1515" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1515" s="1" t="s">
-        <v>1540</v>
+        <v>1541</v>
       </c>
       <c r="B1515" s="1" t="s">
-        <v>1681</v>
+        <v>1692</v>
       </c>
     </row>
     <row r="1516" spans="1:2" x14ac:dyDescent="0.25">
@@ -17890,7 +17887,7 @@
         <v>1542</v>
       </c>
       <c r="B1516" s="1" t="s">
-        <v>1693</v>
+        <v>1677</v>
       </c>
     </row>
     <row r="1517" spans="1:2" x14ac:dyDescent="0.25">
@@ -17898,23 +17895,23 @@
         <v>1543</v>
       </c>
       <c r="B1517" s="1" t="s">
-        <v>1678</v>
-      </c>
-    </row>
-    <row r="1518" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1544</v>
+      </c>
+    </row>
+    <row r="1518" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1518" s="1" t="s">
-        <v>1544</v>
+        <v>1545</v>
       </c>
       <c r="B1518" s="1" t="s">
-        <v>1545</v>
-      </c>
-    </row>
-    <row r="1519" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1546</v>
+      </c>
+    </row>
+    <row r="1519" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1519" s="1" t="s">
-        <v>1546</v>
+        <v>1549</v>
       </c>
       <c r="B1519" s="1" t="s">
-        <v>1547</v>
+        <v>1709</v>
       </c>
     </row>
     <row r="1520" spans="1:2" x14ac:dyDescent="0.25">
@@ -17925,92 +17922,92 @@
         <v>1710</v>
       </c>
     </row>
-    <row r="1521" spans="1:2" x14ac:dyDescent="0.25">
+    <row r="1521" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1521" s="1" t="s">
-        <v>1551</v>
+        <v>1553</v>
       </c>
       <c r="B1521" s="1" t="s">
-        <v>1711</v>
-      </c>
-    </row>
-    <row r="1522" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="1522" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1522" s="1" t="s">
+        <v>1555</v>
+      </c>
+      <c r="B1522" s="1" t="s">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1523" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+      <c r="A1523" s="1" t="s">
+        <v>1557</v>
+      </c>
+      <c r="B1523" s="1" t="s">
         <v>1554</v>
       </c>
-      <c r="B1522" s="1" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="1523" spans="1:2" x14ac:dyDescent="0.25">
-      <c r="A1523" s="1" t="s">
-        <v>1556</v>
-      </c>
-      <c r="B1523" s="1" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="1524" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    </row>
+    <row r="1524" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1524" s="1" t="s">
         <v>1558</v>
       </c>
       <c r="B1524" s="1" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="1525" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1525" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1525" s="1" t="s">
         <v>1559</v>
       </c>
       <c r="B1525" s="1" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="1526" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="1526" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1526" s="1" t="s">
         <v>1560</v>
       </c>
       <c r="B1526" s="1" t="s">
-        <v>1555</v>
-      </c>
-    </row>
-    <row r="1527" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1556</v>
+      </c>
+    </row>
+    <row r="1527" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1527" s="1" t="s">
         <v>1561</v>
       </c>
       <c r="B1527" s="1" t="s">
-        <v>1557</v>
-      </c>
-    </row>
-    <row r="1528" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1554</v>
+      </c>
+    </row>
+    <row r="1528" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1528" s="1" t="s">
         <v>1562</v>
       </c>
       <c r="B1528" s="1" t="s">
-        <v>1555</v>
+        <v>1556</v>
       </c>
     </row>
     <row r="1529" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1529" s="1" t="s">
-        <v>1563</v>
+        <v>1565</v>
       </c>
       <c r="B1529" s="1" t="s">
-        <v>1557</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1530" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1530" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="B1530" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1531" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1531" s="1" t="s">
-        <v>1568</v>
+        <v>1569</v>
       </c>
       <c r="B1531" s="1" t="s">
-        <v>1569</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1532" spans="1:2" x14ac:dyDescent="0.25">
@@ -18018,7 +18015,7 @@
         <v>1570</v>
       </c>
       <c r="B1532" s="1" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1533" spans="1:2" x14ac:dyDescent="0.25">
@@ -18026,7 +18023,7 @@
         <v>1571</v>
       </c>
       <c r="B1533" s="1" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1534" spans="1:2" x14ac:dyDescent="0.25">
@@ -18034,7 +18031,7 @@
         <v>1572</v>
       </c>
       <c r="B1534" s="1" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1535" spans="1:2" x14ac:dyDescent="0.25">
@@ -18042,7 +18039,7 @@
         <v>1573</v>
       </c>
       <c r="B1535" s="1" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1536" spans="1:2" x14ac:dyDescent="0.25">
@@ -18050,7 +18047,7 @@
         <v>1574</v>
       </c>
       <c r="B1536" s="1" t="s">
-        <v>1567</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1537" spans="1:2" x14ac:dyDescent="0.25">
@@ -18058,7 +18055,7 @@
         <v>1575</v>
       </c>
       <c r="B1537" s="1" t="s">
-        <v>1567</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1538" spans="1:2" x14ac:dyDescent="0.25">
@@ -18066,7 +18063,7 @@
         <v>1576</v>
       </c>
       <c r="B1538" s="1" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1539" spans="1:2" x14ac:dyDescent="0.25">
@@ -18074,7 +18071,7 @@
         <v>1577</v>
       </c>
       <c r="B1539" s="1" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1540" spans="1:2" x14ac:dyDescent="0.25">
@@ -18082,7 +18079,7 @@
         <v>1578</v>
       </c>
       <c r="B1540" s="1" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1541" spans="1:2" x14ac:dyDescent="0.25">
@@ -18090,7 +18087,7 @@
         <v>1579</v>
       </c>
       <c r="B1541" s="1" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1542" spans="1:2" x14ac:dyDescent="0.25">
@@ -18098,42 +18095,42 @@
         <v>1580</v>
       </c>
       <c r="B1542" s="1" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1543" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1543" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1543" s="1" t="s">
         <v>1581</v>
       </c>
       <c r="B1543" s="1" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1544" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1674</v>
+      </c>
+    </row>
+    <row r="1544" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1544" s="1" t="s">
         <v>1582</v>
       </c>
       <c r="B1544" s="1" t="s">
-        <v>1675</v>
-      </c>
-    </row>
-    <row r="1545" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1568</v>
+      </c>
+    </row>
+    <row r="1545" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1545" s="1" t="s">
         <v>1583</v>
       </c>
       <c r="B1545" s="1" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1546" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1673</v>
+      </c>
+    </row>
+    <row r="1546" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1546" s="1" t="s">
         <v>1584</v>
       </c>
       <c r="B1546" s="1" t="s">
-        <v>1674</v>
-      </c>
-    </row>
-    <row r="1547" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1670</v>
+      </c>
+    </row>
+    <row r="1547" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1547" s="1" t="s">
         <v>1585</v>
       </c>
@@ -18141,33 +18138,33 @@
         <v>1671</v>
       </c>
     </row>
-    <row r="1548" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+    <row r="1548" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1548" s="1" t="s">
         <v>1586</v>
       </c>
       <c r="B1548" s="1" t="s">
-        <v>1672</v>
-      </c>
-    </row>
-    <row r="1549" spans="1:2" x14ac:dyDescent="0.25">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="1549" spans="1:2" ht="30" x14ac:dyDescent="0.25">
       <c r="A1549" s="1" t="s">
         <v>1587</v>
       </c>
       <c r="B1549" s="1" t="s">
-        <v>1567</v>
-      </c>
-    </row>
-    <row r="1550" spans="1:2" ht="30" x14ac:dyDescent="0.25">
+        <v>1672</v>
+      </c>
+    </row>
+    <row r="1550" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1550" s="1" t="s">
-        <v>1588</v>
+        <v>1565</v>
       </c>
       <c r="B1550" s="1" t="s">
-        <v>1673</v>
+        <v>1731</v>
       </c>
     </row>
     <row r="1551" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1551" s="1" t="s">
-        <v>1566</v>
+        <v>1567</v>
       </c>
       <c r="B1551" s="1" t="s">
         <v>1732</v>
@@ -18175,7 +18172,7 @@
     </row>
     <row r="1552" spans="1:2" x14ac:dyDescent="0.25">
       <c r="A1552" s="1" t="s">
-        <v>1568</v>
+        <v>1588</v>
       </c>
       <c r="B1552" s="1" t="s">
         <v>1733</v>
@@ -18194,7 +18191,7 @@
         <v>1590</v>
       </c>
       <c r="B1554" s="1" t="s">
-        <v>1735</v>
+        <v>1721</v>
       </c>
     </row>
     <row r="1555" spans="1:7" x14ac:dyDescent="0.25">
@@ -18202,7 +18199,7 @@
         <v>1591</v>
       </c>
       <c r="B1555" s="1" t="s">
-        <v>1722</v>
+        <v>1734</v>
       </c>
     </row>
     <row r="1556" spans="1:7" x14ac:dyDescent="0.25">
@@ -18215,7 +18212,7 @@
     </row>
     <row r="1557" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1557" s="1" t="s">
-        <v>1593</v>
+        <v>1520</v>
       </c>
       <c r="B1557" s="1" t="s">
         <v>1736</v>
@@ -18223,10 +18220,10 @@
     </row>
     <row r="1558" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1558" s="1" t="s">
-        <v>1521</v>
+        <v>1593</v>
       </c>
       <c r="B1558" s="1" t="s">
-        <v>1737</v>
+        <v>1736</v>
       </c>
     </row>
     <row r="1559" spans="1:7" x14ac:dyDescent="0.25">
@@ -18234,7 +18231,7 @@
         <v>1594</v>
       </c>
       <c r="B1559" s="1" t="s">
-        <v>1737</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1560" spans="1:7" x14ac:dyDescent="0.25">
@@ -18242,7 +18239,7 @@
         <v>1595</v>
       </c>
       <c r="B1560" s="1" t="s">
-        <v>1569</v>
+        <v>1568</v>
       </c>
     </row>
     <row r="1561" spans="1:7" x14ac:dyDescent="0.25">
@@ -18250,113 +18247,117 @@
         <v>1596</v>
       </c>
       <c r="B1561" s="1" t="s">
-        <v>1569</v>
-      </c>
-    </row>
-    <row r="1562" spans="1:7" x14ac:dyDescent="0.25">
+        <v>1566</v>
+      </c>
+    </row>
+    <row r="1562" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1562" s="1" t="s">
         <v>1597</v>
       </c>
       <c r="B1562" s="1" t="s">
-        <v>1567</v>
-      </c>
-    </row>
-    <row r="1563" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+        <v>1671</v>
+      </c>
+    </row>
+    <row r="1563" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1563" s="1" t="s">
         <v>1598</v>
       </c>
       <c r="B1563" s="1" t="s">
-        <v>1672</v>
+        <v>1566</v>
       </c>
     </row>
     <row r="1564" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1564" s="1" t="s">
-        <v>1599</v>
+        <v>1496</v>
       </c>
       <c r="B1564" s="1" t="s">
-        <v>1567</v>
-      </c>
+        <v>1677</v>
+      </c>
+      <c r="C1564" s="1"/>
+      <c r="D1564" s="1"/>
+      <c r="E1564" s="1"/>
+      <c r="F1564" s="2"/>
     </row>
     <row r="1565" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1565" s="1" t="s">
-        <v>1497</v>
+        <v>1494</v>
       </c>
       <c r="B1565" s="1" t="s">
-        <v>1678</v>
+        <v>1702</v>
       </c>
       <c r="C1565" s="1"/>
       <c r="D1565" s="1"/>
       <c r="E1565" s="1"/>
-      <c r="F1565" s="2"/>
+      <c r="F1565" s="1"/>
     </row>
     <row r="1566" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1566" s="1" t="s">
-        <v>1495</v>
+        <v>1499</v>
       </c>
       <c r="B1566" s="1" t="s">
-        <v>1703</v>
+        <v>1687</v>
       </c>
       <c r="C1566" s="1"/>
       <c r="D1566" s="1"/>
       <c r="E1566" s="1"/>
       <c r="F1566" s="1"/>
-    </row>
-    <row r="1567" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="G1566" s="1"/>
+    </row>
+    <row r="1567" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1567" s="1" t="s">
         <v>1500</v>
       </c>
       <c r="B1567" s="1" t="s">
-        <v>1688</v>
+        <v>1680</v>
       </c>
       <c r="C1567" s="1"/>
       <c r="D1567" s="1"/>
       <c r="E1567" s="1"/>
-      <c r="F1567" s="1"/>
-      <c r="G1567" s="1"/>
-    </row>
-    <row r="1568" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+      <c r="F1567" s="2"/>
+    </row>
+    <row r="1568" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1568" s="1" t="s">
-        <v>1501</v>
+        <v>1489</v>
       </c>
       <c r="B1568" s="1" t="s">
-        <v>1681</v>
+        <v>1708</v>
       </c>
       <c r="C1568" s="1"/>
       <c r="D1568" s="1"/>
       <c r="E1568" s="1"/>
-      <c r="F1568" s="2"/>
-    </row>
-    <row r="1569" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F1568" s="1"/>
+      <c r="G1568" s="1"/>
+    </row>
+    <row r="1569" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1569" s="1" t="s">
-        <v>1490</v>
+        <v>1488</v>
       </c>
       <c r="B1569" s="1" t="s">
-        <v>1709</v>
+        <v>1674</v>
       </c>
       <c r="C1569" s="1"/>
       <c r="D1569" s="1"/>
       <c r="E1569" s="1"/>
       <c r="F1569" s="1"/>
-      <c r="G1569" s="1"/>
     </row>
     <row r="1570" spans="1:7" ht="30" x14ac:dyDescent="0.25">
       <c r="A1570" s="1" t="s">
-        <v>1489</v>
+        <v>1492</v>
       </c>
       <c r="B1570" s="1" t="s">
-        <v>1675</v>
+        <v>1701</v>
       </c>
       <c r="C1570" s="1"/>
       <c r="D1570" s="1"/>
       <c r="E1570" s="1"/>
       <c r="F1570" s="1"/>
     </row>
-    <row r="1571" spans="1:7" ht="30" x14ac:dyDescent="0.25">
+    <row r="1571" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1571" s="1" t="s">
-        <v>1493</v>
+        <v>1490</v>
       </c>
       <c r="B1571" s="1" t="s">
-        <v>1702</v>
+        <v>1710</v>
       </c>
       <c r="C1571" s="1"/>
       <c r="D1571" s="1"/>
@@ -18365,10 +18366,10 @@
     </row>
     <row r="1572" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1572" s="1" t="s">
-        <v>1491</v>
+        <v>1497</v>
       </c>
       <c r="B1572" s="1" t="s">
-        <v>1711</v>
+        <v>1686</v>
       </c>
       <c r="C1572" s="1"/>
       <c r="D1572" s="1"/>
@@ -18377,10 +18378,10 @@
     </row>
     <row r="1573" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1573" s="1" t="s">
-        <v>1498</v>
+        <v>1495</v>
       </c>
       <c r="B1573" s="1" t="s">
-        <v>1687</v>
+        <v>1697</v>
       </c>
       <c r="C1573" s="1"/>
       <c r="D1573" s="1"/>
@@ -18389,22 +18390,23 @@
     </row>
     <row r="1574" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1574" s="1" t="s">
-        <v>1496</v>
+        <v>1493</v>
       </c>
       <c r="B1574" s="1" t="s">
-        <v>1698</v>
+        <v>1699</v>
       </c>
       <c r="C1574" s="1"/>
       <c r="D1574" s="1"/>
       <c r="E1574" s="1"/>
       <c r="F1574" s="1"/>
+      <c r="G1574" s="1"/>
     </row>
     <row r="1575" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1575" s="1" t="s">
-        <v>1494</v>
+        <v>1491</v>
       </c>
       <c r="B1575" s="1" t="s">
-        <v>1700</v>
+        <v>1709</v>
       </c>
       <c r="C1575" s="1"/>
       <c r="D1575" s="1"/>
@@ -18412,12 +18414,12 @@
       <c r="F1575" s="1"/>
       <c r="G1575" s="1"/>
     </row>
-    <row r="1576" spans="1:7" x14ac:dyDescent="0.25">
+    <row r="1576" spans="1:7" ht="45" x14ac:dyDescent="0.25">
       <c r="A1576" s="1" t="s">
-        <v>1492</v>
+        <v>1498</v>
       </c>
       <c r="B1576" s="1" t="s">
-        <v>1710</v>
+        <v>1688</v>
       </c>
       <c r="C1576" s="1"/>
       <c r="D1576" s="1"/>
@@ -18425,37 +18427,32 @@
       <c r="F1576" s="1"/>
       <c r="G1576" s="1"/>
     </row>
-    <row r="1577" spans="1:7" ht="45" x14ac:dyDescent="0.25">
+    <row r="1577" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1577" s="1" t="s">
-        <v>1499</v>
+        <v>1690</v>
       </c>
       <c r="B1577" s="1" t="s">
-        <v>1689</v>
+        <v>1692</v>
       </c>
       <c r="C1577" s="1"/>
       <c r="D1577" s="1"/>
       <c r="E1577" s="1"/>
-      <c r="F1577" s="1"/>
-      <c r="G1577" s="1"/>
+      <c r="F1577" s="2"/>
     </row>
     <row r="1578" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1578" s="1" t="s">
         <v>1691</v>
       </c>
       <c r="B1578" s="1" t="s">
-        <v>1693</v>
-      </c>
-      <c r="C1578" s="1"/>
-      <c r="D1578" s="1"/>
-      <c r="E1578" s="1"/>
-      <c r="F1578" s="2"/>
+        <v>1692</v>
+      </c>
     </row>
     <row r="1579" spans="1:7" x14ac:dyDescent="0.25">
       <c r="A1579" s="1" t="s">
-        <v>1692</v>
+        <v>1737</v>
       </c>
       <c r="B1579" s="1" t="s">
-        <v>1693</v>
+        <v>1737</v>
       </c>
     </row>
     <row r="1580" spans="1:7" x14ac:dyDescent="0.25">
@@ -18490,21 +18487,13 @@
         <v>1741</v>
       </c>
     </row>
-    <row r="1584" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1584" s="1" t="s">
-        <v>1742</v>
-      </c>
-      <c r="B1584" s="1" t="s">
-        <v>1742</v>
-      </c>
-    </row>
   </sheetData>
-  <autoFilter ref="A1:G1579" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
+  <autoFilter ref="A1:G1578" xr:uid="{AE792A93-0F7F-4F11-B4F9-CDC032EF3078}"/>
   <dataConsolidate/>
-  <conditionalFormatting sqref="A1585:B1048576 A1:B1579">
+  <conditionalFormatting sqref="A1584:B1048576 A1:B1578">
     <cfRule type="duplicateValues" dxfId="2" priority="3"/>
   </conditionalFormatting>
-  <conditionalFormatting sqref="A1580:B1584">
+  <conditionalFormatting sqref="A1579:B1583">
     <cfRule type="duplicateValues" dxfId="1" priority="1"/>
     <cfRule type="duplicateValues" dxfId="0" priority="2"/>
   </conditionalFormatting>

</xml_diff>